<commit_message>
Added function to train subtractor with 500 frames
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="134">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -369,6 +369,12 @@
     <t xml:space="preserve">11:30 – 13:30 14:40 – 15:30</t>
   </si>
   <si>
+    <t xml:space="preserve">Speed Estimation + Calibration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:00– 14:30</t>
+  </si>
+  <si>
     <t xml:space="preserve">Design</t>
   </si>
   <si>
@@ -376,6 +382,9 @@
   </si>
   <si>
     <t xml:space="preserve">Percentage Completion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totals</t>
   </si>
   <si>
     <t xml:space="preserve">Value</t>
@@ -421,13 +430,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D\-MMM"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="H:MM"/>
     <numFmt numFmtId="168" formatCode="0.00%"/>
     <numFmt numFmtId="169" formatCode="D/MM/YYYY"/>
+    <numFmt numFmtId="170" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -741,7 +751,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1012,6 +1022,10 @@
     </xf>
     <xf numFmtId="169" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1086,7 +1100,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1252,7 +1266,7 @@
                   <c:v>24.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v/>
@@ -1293,11 +1307,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="48228222"/>
-        <c:axId val="68917907"/>
+        <c:axId val="91430128"/>
+        <c:axId val="90278105"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48228222"/>
+        <c:axId val="91430128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1325,14 +1339,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68917907"/>
+        <c:crossAx val="90278105"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68917907"/>
+        <c:axId val="90278105"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1397,7 +1411,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48228222"/>
+        <c:crossAx val="91430128"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1430,13 +1444,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>1792800</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>348480</xdr:rowOff>
+      <xdr:rowOff>349200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>629640</xdr:colOff>
+      <xdr:colOff>628920</xdr:colOff>
       <xdr:row>78</xdr:row>
-      <xdr:rowOff>179280</xdr:rowOff>
+      <xdr:rowOff>178920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1444,8 +1458,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11089800" y="19588680"/>
-        <a:ext cx="5758920" cy="3238920"/>
+        <a:off x="11089800" y="19589400"/>
+        <a:ext cx="5758200" cy="3236040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1851,10 +1865,8 @@
   </sheetPr>
   <dimension ref="A1:U116"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I65" activeCellId="0" sqref="I65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G75" activeCellId="0" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3274,7 +3286,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="22" t="s">
         <v>27</v>
       </c>
@@ -3285,22 +3297,24 @@
         <v>114</v>
       </c>
       <c r="D74" s="33" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E74" s="33"/>
       <c r="F74" s="33"/>
       <c r="G74" s="34" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="22" t="s">
         <v>29</v>
       </c>
       <c r="B75" s="31" t="n">
         <v>43900</v>
       </c>
-      <c r="C75" s="32"/>
+      <c r="C75" s="32" t="s">
+        <v>116</v>
+      </c>
       <c r="D75" s="33"/>
       <c r="E75" s="33"/>
       <c r="F75" s="33"/>
@@ -3379,7 +3393,7 @@
       <c r="C81" s="32"/>
       <c r="D81" s="33" t="n">
         <f aca="false">SUM(D74:D80)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E81" s="33" t="n">
         <f aca="false">SUM(E74:E80)</f>
@@ -3391,7 +3405,7 @@
       </c>
       <c r="G81" s="33" t="n">
         <f aca="false">SUM(D81:F81)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3426,7 +3440,7 @@
       <c r="B85" s="54"/>
       <c r="C85" s="55"/>
       <c r="D85" s="62" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E85" s="62" t="s">
         <v>25</v>
@@ -3435,21 +3449,21 @@
         <v>26</v>
       </c>
       <c r="G85" s="64" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H85" s="35" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="53"/>
-      <c r="B86" s="58" t="s">
-        <v>42</v>
-      </c>
-      <c r="C86" s="59"/>
+      <c r="B86" s="58"/>
+      <c r="C86" s="59" t="s">
+        <v>120</v>
+      </c>
       <c r="D86" s="63" t="n">
         <f aca="false">SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9)</f>
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E86" s="63" t="n">
         <f aca="false">SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9)</f>
@@ -3461,11 +3475,11 @@
       </c>
       <c r="G86" s="65" t="n">
         <f aca="false">SUM(D86:F86) + 9</f>
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H86" s="66" t="n">
         <f aca="false">G86/400</f>
-        <v>0.41</v>
+        <v>0.4125</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3482,16 +3496,19 @@
       <c r="D88" s="56"/>
       <c r="E88" s="56"/>
       <c r="F88" s="63" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="G88" s="64" t="n">
         <f aca="false">G86*50</f>
-        <v>8200</v>
-      </c>
+        <v>8250</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="68"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="9" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C94" s="9" t="s">
         <v>6</v>
@@ -3584,72 +3601,72 @@
       </c>
       <c r="C104" s="9" t="n">
         <f aca="false">G81</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="9" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C105" s="9"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="9" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C106" s="9"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="9" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C107" s="9"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="9" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C108" s="9"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="9" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C109" s="9"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="9" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C110" s="9"/>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="9" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C111" s="9"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="9" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C112" s="9"/>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="9" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C113" s="9"/>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="9" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C114" s="9"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C115" s="9"/>
     </row>
@@ -3657,6 +3674,9 @@
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <conditionalFormatting sqref="B1:B81">
+    <cfRule type="timePeriod" priority="2" timePeriod="today" dxfId="0"/>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Improved counting/recognition by placing thresh on max distance
Max distance a centroid can appear from its last known position
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="135">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -372,7 +372,10 @@
     <t xml:space="preserve">Speed Estimation + Calibration</t>
   </si>
   <si>
-    <t xml:space="preserve">13:00– 14:30</t>
+    <t xml:space="preserve">13:00– 14:30 19:30 – 20:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improving detection</t>
   </si>
   <si>
     <t xml:space="preserve">Design</t>
@@ -439,7 +442,7 @@
     <numFmt numFmtId="169" formatCode="D/MM/YYYY"/>
     <numFmt numFmtId="170" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -513,6 +516,12 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FFF4B183"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -751,7 +760,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -964,6 +973,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -984,11 +997,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1000,19 +1013,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1020,7 +1033,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1037,6 +1050,17 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1100,7 +1124,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1266,7 +1290,7 @@
                   <c:v>24.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v/>
@@ -1307,11 +1331,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="91430128"/>
-        <c:axId val="90278105"/>
+        <c:axId val="41433231"/>
+        <c:axId val="74057101"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91430128"/>
+        <c:axId val="41433231"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1339,14 +1363,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90278105"/>
+        <c:crossAx val="74057101"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90278105"/>
+        <c:axId val="74057101"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1411,7 +1435,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91430128"/>
+        <c:crossAx val="41433231"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1444,13 +1468,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>1792800</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>349200</xdr:rowOff>
+      <xdr:rowOff>349560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>628920</xdr:colOff>
+      <xdr:colOff>628560</xdr:colOff>
       <xdr:row>78</xdr:row>
-      <xdr:rowOff>178920</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1458,8 +1482,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11089800" y="19589400"/>
-        <a:ext cx="5758200" cy="3236040"/>
+        <a:off x="11089800" y="19589760"/>
+        <a:ext cx="5757840" cy="3235680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1865,8 +1889,8 @@
   </sheetPr>
   <dimension ref="A1:U116"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G75" activeCellId="0" sqref="G75"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C79" activeCellId="0" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3305,20 +3329,24 @@
         <v>115</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B75" s="31" t="n">
+      <c r="B75" s="53" t="n">
         <v>43900</v>
       </c>
       <c r="C75" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="D75" s="33"/>
+      <c r="D75" s="33" t="n">
+        <v>2.5</v>
+      </c>
       <c r="E75" s="33"/>
       <c r="F75" s="33"/>
-      <c r="G75" s="34"/>
+      <c r="G75" s="34" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="22" t="s">
@@ -3386,14 +3414,14 @@
       <c r="G80" s="36"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="53"/>
+      <c r="A81" s="54"/>
       <c r="B81" s="31" t="s">
         <v>42</v>
       </c>
       <c r="C81" s="32"/>
       <c r="D81" s="33" t="n">
         <f aca="false">SUM(D74:D80)</f>
-        <v>4</v>
+        <v>6.5</v>
       </c>
       <c r="E81" s="33" t="n">
         <f aca="false">SUM(E74:E80)</f>
@@ -3405,110 +3433,110 @@
       </c>
       <c r="G81" s="33" t="n">
         <f aca="false">SUM(D81:F81)</f>
-        <v>4</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="53"/>
-      <c r="B82" s="54"/>
-      <c r="C82" s="55"/>
-      <c r="D82" s="56"/>
-      <c r="E82" s="56"/>
-      <c r="F82" s="57"/>
-      <c r="G82" s="56"/>
+      <c r="A82" s="54"/>
+      <c r="B82" s="55"/>
+      <c r="C82" s="56"/>
+      <c r="D82" s="57"/>
+      <c r="E82" s="57"/>
+      <c r="F82" s="58"/>
+      <c r="G82" s="57"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="53"/>
-      <c r="B83" s="58"/>
-      <c r="C83" s="59"/>
-      <c r="D83" s="60"/>
-      <c r="E83" s="60"/>
-      <c r="F83" s="61"/>
-      <c r="G83" s="60"/>
+      <c r="A83" s="54"/>
+      <c r="B83" s="59"/>
+      <c r="C83" s="60"/>
+      <c r="D83" s="61"/>
+      <c r="E83" s="61"/>
+      <c r="F83" s="62"/>
+      <c r="G83" s="61"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="53"/>
-      <c r="B84" s="54"/>
-      <c r="C84" s="55"/>
-      <c r="D84" s="56"/>
-      <c r="E84" s="56"/>
-      <c r="F84" s="57"/>
-      <c r="G84" s="56"/>
+      <c r="A84" s="54"/>
+      <c r="B84" s="55"/>
+      <c r="C84" s="56"/>
+      <c r="D84" s="57"/>
+      <c r="E84" s="57"/>
+      <c r="F84" s="58"/>
+      <c r="G84" s="57"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="53"/>
-      <c r="B85" s="54"/>
-      <c r="C85" s="55"/>
-      <c r="D85" s="62" t="s">
-        <v>117</v>
-      </c>
-      <c r="E85" s="62" t="s">
+      <c r="A85" s="54"/>
+      <c r="B85" s="55"/>
+      <c r="C85" s="56"/>
+      <c r="D85" s="63" t="s">
+        <v>118</v>
+      </c>
+      <c r="E85" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="F85" s="63" t="s">
+      <c r="F85" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="G85" s="64" t="s">
-        <v>118</v>
+      <c r="G85" s="65" t="s">
+        <v>119</v>
       </c>
       <c r="H85" s="35" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="53"/>
-      <c r="B86" s="58"/>
-      <c r="C86" s="59" t="s">
-        <v>120</v>
-      </c>
-      <c r="D86" s="63" t="n">
+      <c r="A86" s="54"/>
+      <c r="B86" s="59"/>
+      <c r="C86" s="60" t="s">
+        <v>121</v>
+      </c>
+      <c r="D86" s="64" t="n">
         <f aca="false">SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9)</f>
-        <v>77</v>
-      </c>
-      <c r="E86" s="63" t="n">
+        <v>79.5</v>
+      </c>
+      <c r="E86" s="64" t="n">
         <f aca="false">SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9)</f>
         <v>76.5</v>
       </c>
-      <c r="F86" s="63" t="n">
+      <c r="F86" s="64" t="n">
         <f aca="false">SUM(F82,F73,F65,F57,F49,F41,F33,F25,F17,F9)</f>
         <v>2.5</v>
       </c>
-      <c r="G86" s="65" t="n">
+      <c r="G86" s="66" t="n">
         <f aca="false">SUM(D86:F86) + 9</f>
-        <v>165</v>
-      </c>
-      <c r="H86" s="66" t="n">
+        <v>167.5</v>
+      </c>
+      <c r="H86" s="67" t="n">
         <f aca="false">G86/400</f>
-        <v>0.4125</v>
+        <v>0.41875</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="54"/>
-      <c r="C87" s="55"/>
-      <c r="D87" s="56"/>
-      <c r="E87" s="56"/>
-      <c r="F87" s="57"/>
-      <c r="G87" s="56"/>
+      <c r="B87" s="55"/>
+      <c r="C87" s="56"/>
+      <c r="D87" s="57"/>
+      <c r="E87" s="57"/>
+      <c r="F87" s="58"/>
+      <c r="G87" s="57"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="54"/>
-      <c r="C88" s="67"/>
-      <c r="D88" s="56"/>
-      <c r="E88" s="56"/>
-      <c r="F88" s="63" t="s">
-        <v>121</v>
-      </c>
-      <c r="G88" s="64" t="n">
+      <c r="B88" s="55"/>
+      <c r="C88" s="68"/>
+      <c r="D88" s="57"/>
+      <c r="E88" s="57"/>
+      <c r="F88" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="G88" s="65" t="n">
         <f aca="false">G86*50</f>
-        <v>8250</v>
+        <v>8375</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="68"/>
+      <c r="B89" s="69"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C94" s="9" t="s">
         <v>6</v>
@@ -3601,72 +3629,72 @@
       </c>
       <c r="C104" s="9" t="n">
         <f aca="false">G81</f>
-        <v>4</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C105" s="9"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C106" s="9"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C107" s="9"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C108" s="9"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C109" s="9"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C110" s="9"/>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C111" s="9"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C112" s="9"/>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C113" s="9"/>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C114" s="9"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C115" s="9"/>
     </row>

</xml_diff>

<commit_message>
Added CheeryTree note taking. Started impl. centroid distance threshing.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="137">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -376,6 +376,12 @@
   </si>
   <si>
     <t xml:space="preserve">Improving detection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00 – 11:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improving Detection + Meeting Kaushik</t>
   </si>
   <si>
     <t xml:space="preserve">Design</t>
@@ -1056,9 +1062,15 @@
         <name val="Calibri"/>
         <charset val="1"/>
         <family val="2"/>
-        <color rgb="FF000000"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF006600"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <colors>
@@ -1124,7 +1136,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1290,7 +1302,7 @@
                   <c:v>24.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.5</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v/>
@@ -1331,11 +1343,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="41433231"/>
-        <c:axId val="74057101"/>
+        <c:axId val="67902343"/>
+        <c:axId val="64963775"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="41433231"/>
+        <c:axId val="67902343"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1363,14 +1375,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74057101"/>
+        <c:crossAx val="64963775"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74057101"/>
+        <c:axId val="64963775"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1435,7 +1447,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41433231"/>
+        <c:crossAx val="67902343"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1468,13 +1480,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>1792800</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>349560</xdr:rowOff>
+      <xdr:rowOff>349920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>628560</xdr:colOff>
+      <xdr:colOff>628200</xdr:colOff>
       <xdr:row>78</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1482,8 +1494,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11089800" y="19589760"/>
-        <a:ext cx="5757840" cy="3235680"/>
+        <a:off x="11089800" y="19590120"/>
+        <a:ext cx="5757480" cy="3233880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1890,7 +1902,7 @@
   <dimension ref="A1:U116"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C79" activeCellId="0" sqref="C79"/>
+      <selection pane="topLeft" activeCell="D77" activeCellId="0" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3348,18 +3360,24 @@
         <v>117</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="22" t="s">
         <v>31</v>
       </c>
       <c r="B76" s="31" t="n">
         <v>43901</v>
       </c>
-      <c r="C76" s="32"/>
-      <c r="D76" s="33"/>
+      <c r="C76" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="D76" s="33" t="n">
+        <v>2</v>
+      </c>
       <c r="E76" s="33"/>
       <c r="F76" s="33"/>
-      <c r="G76" s="34"/>
+      <c r="G76" s="34" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="22" t="s">
@@ -3421,7 +3439,7 @@
       <c r="C81" s="32"/>
       <c r="D81" s="33" t="n">
         <f aca="false">SUM(D74:D80)</f>
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
       <c r="E81" s="33" t="n">
         <f aca="false">SUM(E74:E80)</f>
@@ -3433,7 +3451,7 @@
       </c>
       <c r="G81" s="33" t="n">
         <f aca="false">SUM(D81:F81)</f>
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3468,7 +3486,7 @@
       <c r="B85" s="55"/>
       <c r="C85" s="56"/>
       <c r="D85" s="63" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E85" s="63" t="s">
         <v>25</v>
@@ -3477,21 +3495,21 @@
         <v>26</v>
       </c>
       <c r="G85" s="65" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H85" s="35" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="54"/>
       <c r="B86" s="59"/>
       <c r="C86" s="60" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D86" s="64" t="n">
         <f aca="false">SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9)</f>
-        <v>79.5</v>
+        <v>81.5</v>
       </c>
       <c r="E86" s="64" t="n">
         <f aca="false">SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9)</f>
@@ -3503,11 +3521,11 @@
       </c>
       <c r="G86" s="66" t="n">
         <f aca="false">SUM(D86:F86) + 9</f>
-        <v>167.5</v>
+        <v>169.5</v>
       </c>
       <c r="H86" s="67" t="n">
         <f aca="false">G86/400</f>
-        <v>0.41875</v>
+        <v>0.42375</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3524,11 +3542,11 @@
       <c r="D88" s="57"/>
       <c r="E88" s="57"/>
       <c r="F88" s="64" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="G88" s="65" t="n">
         <f aca="false">G86*50</f>
-        <v>8375</v>
+        <v>8475</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3536,7 +3554,7 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C94" s="9" t="s">
         <v>6</v>
@@ -3629,72 +3647,72 @@
       </c>
       <c r="C104" s="9" t="n">
         <f aca="false">G81</f>
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="9" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C105" s="9"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="9" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C106" s="9"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C107" s="9"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="9" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C108" s="9"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="9" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C109" s="9"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C110" s="9"/>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="9" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C111" s="9"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C112" s="9"/>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C113" s="9"/>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="9" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C114" s="9"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="9" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C115" s="9"/>
     </row>

</xml_diff>

<commit_message>
Added improved centroid generation with threshing.
- Need to more vigorously test to verify it's behaving correctly.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -378,10 +378,10 @@
     <t xml:space="preserve">Improving detection</t>
   </si>
   <si>
-    <t xml:space="preserve">9:00 – 11:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Improving Detection + Meeting Kaushik</t>
+    <t xml:space="preserve">9:00 – 11:00 11:30 – 12:00 13:00 – 15:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improving Detection + Meeting Kaushik + Improving Centroid Detection</t>
   </si>
   <si>
     <t xml:space="preserve">Design</t>
@@ -807,10 +807,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -839,10 +835,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -891,6 +883,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -904,15 +900,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -932,7 +928,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -952,7 +948,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -975,6 +971,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1003,6 +1003,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1027,12 +1031,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -1136,7 +1136,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1302,7 +1302,7 @@
                   <c:v>24.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v/>
@@ -1343,11 +1343,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="67902343"/>
-        <c:axId val="64963775"/>
+        <c:axId val="77470976"/>
+        <c:axId val="9002944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="67902343"/>
+        <c:axId val="77470976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1375,14 +1375,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64963775"/>
+        <c:crossAx val="9002944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64963775"/>
+        <c:axId val="9002944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1447,7 +1447,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67902343"/>
+        <c:crossAx val="77470976"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1480,13 +1480,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>1792800</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>349920</xdr:rowOff>
+      <xdr:rowOff>350640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>628200</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>7920</xdr:rowOff>
+      <xdr:colOff>627840</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>49680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1494,8 +1494,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11089800" y="19590120"/>
-        <a:ext cx="5757480" cy="3233880"/>
+        <a:off x="11089800" y="18259200"/>
+        <a:ext cx="5757120" cy="3079800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1899,272 +1899,272 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U116"/>
+  <dimension ref="A1:U115"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D77" activeCellId="0" sqref="D77"/>
+      <selection pane="topLeft" activeCell="G76" activeCellId="0" sqref="G76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="15.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="9" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="9" width="7.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="10" width="45.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="9" style="11" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="12" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="13" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="8" width="45.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="10" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="9" style="10" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="11" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="12" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="19"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="17"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="23" t="n">
+      <c r="B2" s="21" t="n">
         <v>43836</v>
       </c>
-      <c r="C2" s="24"/>
+      <c r="C2" s="22"/>
       <c r="E2" s="9" t="n">
         <v>1</v>
       </c>
       <c r="F2" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="19"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="I2" s="17"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="17"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="23" t="n">
+      <c r="B3" s="21" t="n">
         <v>43837</v>
       </c>
-      <c r="C3" s="24"/>
+      <c r="C3" s="22"/>
       <c r="D3" s="9" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="9" t="n">
         <v>0.5</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="19"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
+      <c r="I3" s="17"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="17"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="23" t="n">
+      <c r="B4" s="21" t="n">
         <v>43838</v>
       </c>
-      <c r="C4" s="24"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="9" t="n">
         <v>3</v>
       </c>
       <c r="E4" s="9" t="n">
         <v>0.5</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="25"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="19"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="s">
+      <c r="I4" s="23"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="17"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="23" t="n">
+      <c r="B5" s="21" t="n">
         <v>43839</v>
       </c>
-      <c r="C5" s="24"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="9" t="n">
         <v>5</v>
       </c>
       <c r="E5" s="9" t="n">
         <v>0.5</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="25"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="19"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="s">
+      <c r="I5" s="23"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="17"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="23" t="n">
+      <c r="B6" s="21" t="n">
         <v>43840</v>
       </c>
-      <c r="C6" s="24"/>
+      <c r="C6" s="22"/>
       <c r="D6" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="25"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="19"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22" t="s">
+      <c r="I6" s="23"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="17"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="23" t="n">
+      <c r="B7" s="21" t="n">
         <v>43841</v>
       </c>
-      <c r="C7" s="24"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="25"/>
-      <c r="U7" s="19"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="s">
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="17"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="23" t="n">
+      <c r="B8" s="21" t="n">
         <v>43842</v>
       </c>
-      <c r="C8" s="24"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="25"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="19"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
+      <c r="I8" s="23"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="17"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="28" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -2182,270 +2182,270 @@
         <f aca="false">SUM(F2:F8)</f>
         <v>1</v>
       </c>
-      <c r="G9" s="9" t="n">
+      <c r="G9" s="29" t="n">
         <f aca="false">SUM(D9:F9)</f>
         <v>18.5</v>
       </c>
-      <c r="I9" s="25"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="19"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22" t="s">
+      <c r="I9" s="23"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="17"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="31" t="n">
+      <c r="B10" s="30" t="n">
         <v>43843</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="33" t="n">
+      <c r="C10" s="31"/>
+      <c r="D10" s="32" t="n">
         <v>4</v>
       </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="34" t="s">
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="25"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22" t="s">
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="23"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="31" t="n">
+      <c r="B11" s="30" t="n">
         <v>43844</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="33" t="n">
+      <c r="C11" s="31"/>
+      <c r="D11" s="32" t="n">
         <v>1</v>
       </c>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="34" t="s">
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="33" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="31" t="n">
+      <c r="B12" s="30" t="n">
         <v>43845</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="33" t="n">
+      <c r="C12" s="31"/>
+      <c r="D12" s="32" t="n">
         <v>2</v>
       </c>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="34" t="s">
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="35"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22" t="s">
+      <c r="H12" s="34"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="31" t="n">
+      <c r="B13" s="30" t="n">
         <v>43846</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="33" t="n">
+      <c r="C13" s="31"/>
+      <c r="D13" s="32" t="n">
         <v>4</v>
       </c>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="34" t="s">
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="33" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="22" t="s">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="31" t="n">
+      <c r="B14" s="30" t="n">
         <v>43847</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="36"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="22" t="s">
+      <c r="C14" s="31"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="31"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="31" t="n">
+      <c r="B15" s="30" t="n">
         <v>43848</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="36"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="22" t="s">
+      <c r="C15" s="31"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="31"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="31" t="n">
+      <c r="B16" s="30" t="n">
         <v>43849</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="36"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="30" t="s">
+      <c r="C16" s="31"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="31"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="33" t="n">
+      <c r="C17" s="31"/>
+      <c r="D17" s="32" t="n">
         <f aca="false">SUM(D10:D16)</f>
         <v>11</v>
       </c>
-      <c r="E17" s="33" t="n">
+      <c r="E17" s="32" t="n">
         <f aca="false">SUM(E10:E16)</f>
         <v>0</v>
       </c>
-      <c r="F17" s="33" t="n">
+      <c r="F17" s="32" t="n">
         <f aca="false">SUM(F10:F16)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="33" t="n">
+      <c r="G17" s="35" t="n">
         <f aca="false">SUM(D17:F17)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="22" t="s">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="23" t="n">
+      <c r="B18" s="21" t="n">
         <v>43850</v>
       </c>
-      <c r="C18" s="24"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="22" t="s">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="23" t="n">
+      <c r="B19" s="21" t="n">
         <v>43851</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="22" t="s">
         <v>49</v>
       </c>
       <c r="D19" s="9" t="n">
         <v>3.5</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="38" t="n">
+      <c r="B20" s="37" t="n">
         <v>43852</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="22" t="s">
         <v>51</v>
       </c>
       <c r="D20" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="22" t="s">
+    <row r="21" customFormat="false" ht="55.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="23" t="n">
+      <c r="B21" s="21" t="n">
         <v>43853</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="22" t="s">
         <v>53</v>
       </c>
       <c r="E21" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="H21" s="39" t="s">
+      <c r="H21" s="38" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="22" t="s">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="23" t="n">
+      <c r="B22" s="21" t="n">
         <v>43854</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="22" t="s">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="23" t="n">
+      <c r="B23" s="21" t="n">
         <v>43855</v>
       </c>
-      <c r="C23" s="24"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="22" t="s">
+      <c r="C23" s="22"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="23" t="n">
+      <c r="B24" s="21" t="n">
         <v>43856</v>
       </c>
-      <c r="C24" s="24"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="30" t="s">
+      <c r="C24" s="22"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="28" t="s">
         <v>57</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -2459,271 +2459,271 @@
         <f aca="false">SUM(E18:E24)</f>
         <v>5</v>
       </c>
-      <c r="G25" s="9" t="n">
+      <c r="G25" s="29" t="n">
         <f aca="false">SUM(D25:F25)</f>
         <v>17.5</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="22" t="s">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="31" t="n">
+      <c r="B26" s="30" t="n">
         <v>43857</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33" t="n">
+      <c r="D26" s="32"/>
+      <c r="E26" s="32" t="n">
         <v>1.5</v>
       </c>
-      <c r="F26" s="33"/>
-      <c r="G26" s="34" t="s">
+      <c r="F26" s="32"/>
+      <c r="G26" s="33" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="22" t="s">
+    <row r="27" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="31" t="n">
+      <c r="B27" s="30" t="n">
         <v>43858</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="40"/>
-      <c r="E27" s="33" t="n">
+      <c r="D27" s="39"/>
+      <c r="E27" s="32" t="n">
         <v>4.5</v>
       </c>
-      <c r="F27" s="33"/>
-      <c r="G27" s="34" t="s">
+      <c r="F27" s="32"/>
+      <c r="G27" s="33" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="22" t="s">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="31" t="n">
+      <c r="B28" s="30" t="n">
         <v>43859</v>
       </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="34"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="22" t="s">
+      <c r="C28" s="31"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="33"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="31" t="n">
+      <c r="B29" s="30" t="n">
         <v>43860</v>
       </c>
-      <c r="C29" s="32"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="41"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="22" t="s">
+      <c r="C29" s="31"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="40"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="31" t="n">
+      <c r="B30" s="30" t="n">
         <v>43861</v>
       </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="36"/>
-    </row>
-    <row r="31" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="22" t="s">
+      <c r="C30" s="31"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="31"/>
+    </row>
+    <row r="31" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="31" t="n">
+      <c r="B31" s="30" t="n">
         <v>43862</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33" t="n">
+      <c r="D31" s="32"/>
+      <c r="E31" s="32" t="n">
         <v>3</v>
       </c>
-      <c r="F31" s="33"/>
-      <c r="G31" s="36" t="s">
+      <c r="F31" s="32"/>
+      <c r="G31" s="31" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="22" t="s">
+    <row r="32" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="31" t="n">
+      <c r="B32" s="30" t="n">
         <v>43863</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33" t="n">
+      <c r="D32" s="32"/>
+      <c r="E32" s="32" t="n">
         <v>3</v>
       </c>
-      <c r="F32" s="33"/>
-      <c r="G32" s="36" t="s">
+      <c r="F32" s="32"/>
+      <c r="G32" s="31" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="30" t="s">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="32"/>
-      <c r="D33" s="33" t="n">
+      <c r="C33" s="31"/>
+      <c r="D33" s="32" t="n">
         <f aca="false">SUM(D26:D32)</f>
         <v>0</v>
       </c>
-      <c r="E33" s="33" t="n">
+      <c r="E33" s="32" t="n">
         <f aca="false">SUM(E26:E32)</f>
         <v>12</v>
       </c>
-      <c r="F33" s="33" t="n">
+      <c r="F33" s="32" t="n">
         <v>0</v>
       </c>
-      <c r="G33" s="33" t="n">
+      <c r="G33" s="35" t="n">
         <f aca="false">SUM(D33:F33)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="22" t="s">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="23" t="n">
+      <c r="B34" s="21" t="n">
         <v>43864</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="22" t="s">
         <v>63</v>
       </c>
       <c r="E34" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="G34" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="22" t="s">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="23" t="n">
+      <c r="B35" s="21" t="n">
         <v>43865</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="22" t="s">
         <v>64</v>
       </c>
       <c r="E35" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="G35" s="10" t="s">
+      <c r="G35" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="22" t="s">
+    <row r="36" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="23" t="n">
+      <c r="B36" s="21" t="n">
         <v>43866</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="22" t="s">
         <v>65</v>
       </c>
       <c r="E36" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="G36" s="10" t="s">
+      <c r="G36" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="22" t="s">
+    <row r="37" customFormat="false" ht="55.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="23" t="n">
+      <c r="B37" s="21" t="n">
         <v>43867</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="22" t="s">
         <v>66</v>
       </c>
       <c r="E37" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="G37" s="10" t="s">
+      <c r="G37" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="22" t="s">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="23" t="n">
+      <c r="B38" s="21" t="n">
         <v>43868</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="22" t="s">
         <v>68</v>
       </c>
       <c r="E38" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="G38" s="10" t="s">
+      <c r="G38" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="22" t="s">
+    <row r="39" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="23" t="n">
+      <c r="B39" s="21" t="n">
         <v>43869</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="22" t="s">
         <v>69</v>
       </c>
       <c r="E39" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="G39" s="10" t="s">
+      <c r="G39" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="22" t="s">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="23" t="n">
+      <c r="B40" s="21" t="n">
         <v>43870</v>
       </c>
-      <c r="C40" s="24" t="s">
+      <c r="C40" s="22" t="s">
         <v>70</v>
       </c>
       <c r="E40" s="9" t="n">
         <v>3.5</v>
       </c>
-      <c r="G40" s="10" t="s">
+      <c r="G40" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="30" t="s">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="28" t="s">
         <v>71</v>
       </c>
       <c r="B41" s="7" t="s">
@@ -2737,267 +2737,267 @@
         <f aca="false">SUM(E34:E40)</f>
         <v>22.5</v>
       </c>
-      <c r="G41" s="9" t="n">
+      <c r="G41" s="29" t="n">
         <f aca="false">SUM(D41:F41)</f>
         <v>22.5</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="22" t="s">
+    <row r="42" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="31" t="n">
+      <c r="B42" s="30" t="n">
         <v>43871</v>
       </c>
-      <c r="C42" s="32" t="s">
+      <c r="C42" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="D42" s="33"/>
-      <c r="E42" s="33" t="n">
+      <c r="D42" s="32"/>
+      <c r="E42" s="32" t="n">
         <v>3.5</v>
       </c>
-      <c r="F42" s="33"/>
-      <c r="G42" s="34" t="s">
+      <c r="F42" s="32"/>
+      <c r="G42" s="33" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="22" t="s">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B43" s="31" t="n">
+      <c r="B43" s="30" t="n">
         <v>43872</v>
       </c>
-      <c r="C43" s="32"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="34"/>
-    </row>
-    <row r="44" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="22" t="s">
+      <c r="C43" s="31"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="33"/>
+    </row>
+    <row r="44" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="31" t="n">
+      <c r="B44" s="30" t="n">
         <v>43873</v>
       </c>
-      <c r="C44" s="32" t="s">
+      <c r="C44" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="D44" s="33"/>
-      <c r="E44" s="33" t="n">
+      <c r="D44" s="32"/>
+      <c r="E44" s="32" t="n">
         <v>3</v>
       </c>
-      <c r="F44" s="33"/>
-      <c r="G44" s="34" t="s">
+      <c r="F44" s="32"/>
+      <c r="G44" s="33" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="22" t="s">
+    <row r="45" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B45" s="31" t="n">
+      <c r="B45" s="30" t="n">
         <v>43874</v>
       </c>
-      <c r="C45" s="32" t="s">
+      <c r="C45" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="D45" s="33"/>
-      <c r="E45" s="33" t="n">
+      <c r="D45" s="32"/>
+      <c r="E45" s="32" t="n">
         <v>4.5</v>
       </c>
-      <c r="F45" s="33"/>
-      <c r="G45" s="34" t="s">
+      <c r="F45" s="32"/>
+      <c r="G45" s="33" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="22" t="s">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B46" s="31" t="n">
+      <c r="B46" s="30" t="n">
         <v>43875</v>
       </c>
-      <c r="C46" s="32"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="36"/>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="22" t="s">
+      <c r="C46" s="31"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="31"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="31" t="n">
+      <c r="B47" s="30" t="n">
         <v>43876</v>
       </c>
-      <c r="C47" s="32"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="36"/>
-    </row>
-    <row r="48" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="22" t="s">
+      <c r="C47" s="31"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="31"/>
+    </row>
+    <row r="48" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="31" t="n">
+      <c r="B48" s="30" t="n">
         <v>43877</v>
       </c>
-      <c r="C48" s="32" t="s">
+      <c r="C48" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="D48" s="33"/>
-      <c r="E48" s="33" t="n">
+      <c r="D48" s="32"/>
+      <c r="E48" s="32" t="n">
         <v>2.5</v>
       </c>
-      <c r="F48" s="33"/>
-      <c r="G48" s="36" t="s">
+      <c r="F48" s="32"/>
+      <c r="G48" s="31" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="30" t="s">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="B49" s="31" t="s">
+      <c r="B49" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C49" s="32"/>
-      <c r="D49" s="33"/>
-      <c r="E49" s="33" t="n">
+      <c r="C49" s="31"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32" t="n">
         <f aca="false">SUM(E42:E48)</f>
         <v>13.5</v>
       </c>
-      <c r="F49" s="33"/>
-      <c r="G49" s="33" t="n">
+      <c r="F49" s="32"/>
+      <c r="G49" s="35" t="n">
         <f aca="false">SUM(D49,E49,F49)</f>
         <v>13.5</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="22" t="s">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="23" t="n">
+      <c r="B50" s="21" t="n">
         <v>43878</v>
       </c>
-      <c r="C50" s="24" t="s">
+      <c r="C50" s="22" t="s">
         <v>77</v>
       </c>
       <c r="E50" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="G50" s="10" t="s">
+      <c r="G50" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="22" t="s">
+    <row r="51" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B51" s="23" t="n">
+      <c r="B51" s="21" t="n">
         <v>43879</v>
       </c>
-      <c r="C51" s="24" t="s">
+      <c r="C51" s="22" t="s">
         <v>79</v>
       </c>
       <c r="E51" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="G51" s="10" t="s">
+      <c r="G51" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="22" t="s">
+    <row r="52" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B52" s="23" t="n">
+      <c r="B52" s="21" t="n">
         <v>43880</v>
       </c>
-      <c r="C52" s="24" t="s">
+      <c r="C52" s="22" t="s">
         <v>81</v>
       </c>
       <c r="E52" s="9" t="n">
         <v>4.5</v>
       </c>
-      <c r="G52" s="10" t="s">
+      <c r="G52" s="8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="22" t="s">
+    <row r="53" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B53" s="23" t="n">
+      <c r="B53" s="21" t="n">
         <v>43881</v>
       </c>
-      <c r="C53" s="42" t="s">
+      <c r="C53" s="41" t="s">
         <v>83</v>
       </c>
       <c r="E53" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="G53" s="10" t="s">
+      <c r="G53" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="22" t="s">
+    <row r="54" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B54" s="23" t="n">
+      <c r="B54" s="21" t="n">
         <v>43882</v>
       </c>
-      <c r="C54" s="42" t="s">
+      <c r="C54" s="41" t="s">
         <v>85</v>
       </c>
       <c r="E54" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="G54" s="10" t="s">
+      <c r="G54" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="22" t="s">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B55" s="43" t="n">
+      <c r="B55" s="42" t="n">
         <v>43883</v>
       </c>
-      <c r="C55" s="44" t="s">
+      <c r="C55" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="D55" s="45" t="n">
+      <c r="D55" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="E55" s="45"/>
-      <c r="F55" s="45"/>
-      <c r="G55" s="46" t="s">
+      <c r="E55" s="44"/>
+      <c r="F55" s="44"/>
+      <c r="G55" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="H55" s="47"/>
-      <c r="I55" s="47"/>
-      <c r="J55" s="47"/>
-      <c r="K55" s="47"/>
-      <c r="L55" s="47"/>
-      <c r="M55" s="47"/>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="22" t="s">
+      <c r="H55" s="46"/>
+      <c r="I55" s="46"/>
+      <c r="J55" s="46"/>
+      <c r="K55" s="46"/>
+      <c r="L55" s="46"/>
+      <c r="M55" s="46"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B56" s="23" t="n">
+      <c r="B56" s="21" t="n">
         <v>43884</v>
       </c>
-      <c r="C56" s="24"/>
-      <c r="N56" s="48"/>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="30" t="s">
+      <c r="C56" s="22"/>
+      <c r="N56" s="47"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="28" t="s">
         <v>89</v>
       </c>
       <c r="B57" s="7" t="s">
@@ -3011,160 +3011,160 @@
         <f aca="false">SUM(E50:E56)</f>
         <v>19.5</v>
       </c>
-      <c r="G57" s="9" t="n">
+      <c r="G57" s="29" t="n">
         <f aca="false">SUM(D57:F57)</f>
         <v>20.5</v>
       </c>
-      <c r="N57" s="48"/>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="22" t="s">
+      <c r="N57" s="47"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B58" s="31" t="n">
+      <c r="B58" s="30" t="n">
         <v>43885</v>
       </c>
-      <c r="C58" s="32" t="s">
+      <c r="C58" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="D58" s="33" t="n">
+      <c r="D58" s="32" t="n">
         <v>1.5</v>
       </c>
-      <c r="E58" s="33"/>
-      <c r="F58" s="33" t="n">
+      <c r="E58" s="32"/>
+      <c r="F58" s="32" t="n">
         <v>1.5</v>
       </c>
-      <c r="G58" s="34" t="s">
+      <c r="G58" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="I58" s="11" t="s">
+      <c r="I58" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="N58" s="48"/>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="22" t="s">
+      <c r="N58" s="47"/>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B59" s="31" t="n">
+      <c r="B59" s="30" t="n">
         <v>43886</v>
       </c>
-      <c r="C59" s="32"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="33" t="n">
+      <c r="C59" s="31"/>
+      <c r="D59" s="32"/>
+      <c r="E59" s="32" t="n">
         <v>0.5</v>
       </c>
-      <c r="F59" s="33"/>
-      <c r="G59" s="34"/>
-      <c r="N59" s="48"/>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="22" t="s">
+      <c r="F59" s="32"/>
+      <c r="G59" s="33"/>
+      <c r="N59" s="47"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B60" s="31" t="n">
+      <c r="B60" s="30" t="n">
         <v>43887</v>
       </c>
-      <c r="C60" s="32"/>
-      <c r="D60" s="33" t="n">
+      <c r="C60" s="31"/>
+      <c r="D60" s="32" t="n">
         <v>1</v>
       </c>
-      <c r="E60" s="33" t="n">
+      <c r="E60" s="32" t="n">
         <v>0.5</v>
       </c>
-      <c r="F60" s="33"/>
-      <c r="G60" s="34" t="s">
+      <c r="F60" s="32"/>
+      <c r="G60" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="N60" s="48"/>
-    </row>
-    <row r="61" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="22" t="s">
+      <c r="N60" s="47"/>
+    </row>
+    <row r="61" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B61" s="31" t="n">
+      <c r="B61" s="30" t="n">
         <v>43888</v>
       </c>
-      <c r="C61" s="32" t="s">
+      <c r="C61" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D61" s="33" t="n">
+      <c r="D61" s="32" t="n">
         <v>3.5</v>
       </c>
-      <c r="E61" s="33" t="n">
+      <c r="E61" s="32" t="n">
         <v>0.5</v>
       </c>
-      <c r="F61" s="33"/>
-      <c r="G61" s="41" t="s">
+      <c r="F61" s="32"/>
+      <c r="G61" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="N61" s="48"/>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="22" t="s">
+      <c r="N61" s="47"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B62" s="31" t="n">
+      <c r="B62" s="30" t="n">
         <v>43889</v>
       </c>
-      <c r="C62" s="32"/>
-      <c r="D62" s="33"/>
-      <c r="E62" s="33"/>
-      <c r="F62" s="33"/>
-      <c r="G62" s="36"/>
-      <c r="N62" s="48"/>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="22" t="s">
+      <c r="C62" s="31"/>
+      <c r="D62" s="32"/>
+      <c r="E62" s="32"/>
+      <c r="F62" s="32"/>
+      <c r="G62" s="31"/>
+      <c r="N62" s="47"/>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B63" s="31" t="n">
+      <c r="B63" s="30" t="n">
         <v>43890</v>
       </c>
-      <c r="C63" s="32"/>
-      <c r="D63" s="33"/>
-      <c r="E63" s="33"/>
-      <c r="F63" s="33"/>
-      <c r="G63" s="36"/>
-      <c r="N63" s="48"/>
-    </row>
-    <row r="64" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="22" t="s">
+      <c r="C63" s="31"/>
+      <c r="D63" s="32"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="32"/>
+      <c r="G63" s="31"/>
+      <c r="N63" s="47"/>
+    </row>
+    <row r="64" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B64" s="31" t="n">
+      <c r="B64" s="30" t="n">
         <v>43891</v>
       </c>
-      <c r="C64" s="32" t="s">
+      <c r="C64" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="D64" s="33" t="n">
+      <c r="D64" s="32" t="n">
         <v>3</v>
       </c>
-      <c r="E64" s="33"/>
-      <c r="F64" s="33"/>
-      <c r="G64" s="36" t="s">
+      <c r="E64" s="32"/>
+      <c r="F64" s="32"/>
+      <c r="G64" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="N64" s="48"/>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="30" t="s">
+      <c r="N64" s="47"/>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="B65" s="49" t="s">
+      <c r="B65" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C65" s="50"/>
-      <c r="D65" s="51" t="n">
+      <c r="C65" s="49"/>
+      <c r="D65" s="50" t="n">
         <f aca="false">SUM(D58:D64)</f>
         <v>9</v>
       </c>
-      <c r="E65" s="51" t="n">
+      <c r="E65" s="50" t="n">
         <f aca="false">SUM(E58:E64)</f>
         <v>1.5</v>
       </c>
-      <c r="F65" s="51" t="n">
+      <c r="F65" s="50" t="n">
         <f aca="false">SUM(F58:F64)</f>
         <v>1.5</v>
       </c>
@@ -3179,96 +3179,96 @@
       <c r="L65" s="52"/>
       <c r="M65" s="52"/>
     </row>
-    <row r="66" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="22" t="s">
+    <row r="66" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B66" s="23" t="n">
+      <c r="B66" s="21" t="n">
         <v>43892</v>
       </c>
-      <c r="C66" s="24" t="s">
+      <c r="C66" s="22" t="s">
         <v>99</v>
       </c>
       <c r="D66" s="9" t="n">
         <v>4.5</v>
       </c>
-      <c r="G66" s="10" t="s">
+      <c r="G66" s="8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="22" t="s">
+    <row r="67" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B67" s="23" t="n">
+      <c r="B67" s="21" t="n">
         <v>43893</v>
       </c>
-      <c r="C67" s="24" t="s">
+      <c r="C67" s="22" t="s">
         <v>101</v>
       </c>
       <c r="D67" s="9" t="n">
         <v>4.5</v>
       </c>
-      <c r="G67" s="10" t="s">
+      <c r="G67" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="22" t="s">
+    <row r="68" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B68" s="23" t="n">
+      <c r="B68" s="21" t="n">
         <v>43894</v>
       </c>
-      <c r="C68" s="24" t="s">
+      <c r="C68" s="22" t="s">
         <v>103</v>
       </c>
       <c r="D68" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="G68" s="10" t="s">
+      <c r="G68" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="22" t="s">
+    <row r="69" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B69" s="23" t="n">
+      <c r="B69" s="21" t="n">
         <v>43895</v>
       </c>
-      <c r="C69" s="24" t="s">
+      <c r="C69" s="22" t="s">
         <v>105</v>
       </c>
       <c r="D69" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="G69" s="10" t="s">
+      <c r="G69" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="22" t="s">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B70" s="23" t="n">
+      <c r="B70" s="21" t="n">
         <v>43896</v>
       </c>
-      <c r="C70" s="24" t="s">
+      <c r="C70" s="22" t="s">
         <v>107</v>
       </c>
       <c r="D70" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="G70" s="10" t="s">
+      <c r="G70" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="22" t="s">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B71" s="23" t="n">
+      <c r="B71" s="21" t="n">
         <v>43897</v>
       </c>
       <c r="C71" s="8" t="s">
@@ -3277,29 +3277,29 @@
       <c r="D71" s="9" t="n">
         <v>1.5</v>
       </c>
-      <c r="G71" s="10" t="s">
+      <c r="G71" s="8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="22" t="s">
+    <row r="72" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B72" s="23" t="n">
+      <c r="B72" s="21" t="n">
         <v>43898</v>
       </c>
-      <c r="C72" s="24" t="s">
+      <c r="C72" s="22" t="s">
         <v>111</v>
       </c>
       <c r="D72" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="G72" s="10" t="s">
+      <c r="G72" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="30" t="s">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="28" t="s">
         <v>113</v>
       </c>
       <c r="B73" s="7" t="s">
@@ -3317,236 +3317,236 @@
         <f aca="false">SUM(F66:F72)</f>
         <v>0</v>
       </c>
-      <c r="G73" s="9" t="n">
+      <c r="G73" s="29" t="n">
         <f aca="false">SUM(D73:F73)</f>
         <v>24.5</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="22" t="s">
+      <c r="A74" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B74" s="31" t="n">
+      <c r="B74" s="30" t="n">
         <v>43899</v>
       </c>
-      <c r="C74" s="32" t="s">
+      <c r="C74" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="D74" s="33" t="n">
+      <c r="D74" s="32" t="n">
         <v>4</v>
       </c>
-      <c r="E74" s="33"/>
-      <c r="F74" s="33"/>
-      <c r="G74" s="34" t="s">
+      <c r="E74" s="32"/>
+      <c r="F74" s="32"/>
+      <c r="G74" s="33" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="22" t="s">
+    <row r="75" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="20" t="s">
         <v>29</v>
       </c>
       <c r="B75" s="53" t="n">
         <v>43900</v>
       </c>
-      <c r="C75" s="32" t="s">
+      <c r="C75" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="D75" s="33" t="n">
+      <c r="D75" s="32" t="n">
         <v>2.5</v>
       </c>
-      <c r="E75" s="33"/>
-      <c r="F75" s="33"/>
-      <c r="G75" s="34" t="s">
+      <c r="E75" s="32"/>
+      <c r="F75" s="32"/>
+      <c r="G75" s="33" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="22" t="s">
+    <row r="76" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B76" s="31" t="n">
+      <c r="B76" s="30" t="n">
         <v>43901</v>
       </c>
-      <c r="C76" s="32" t="s">
+      <c r="C76" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="D76" s="33" t="n">
-        <v>2</v>
-      </c>
-      <c r="E76" s="33"/>
-      <c r="F76" s="33"/>
-      <c r="G76" s="34" t="s">
+      <c r="D76" s="32" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E76" s="32"/>
+      <c r="F76" s="32"/>
+      <c r="G76" s="33" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="22" t="s">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B77" s="31" t="n">
+      <c r="B77" s="30" t="n">
         <v>43902</v>
       </c>
-      <c r="C77" s="32"/>
-      <c r="D77" s="33"/>
-      <c r="E77" s="33"/>
-      <c r="F77" s="33"/>
-      <c r="G77" s="41"/>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="22" t="s">
+      <c r="C77" s="31"/>
+      <c r="D77" s="32"/>
+      <c r="E77" s="32"/>
+      <c r="F77" s="32"/>
+      <c r="G77" s="40"/>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B78" s="31" t="n">
+      <c r="B78" s="30" t="n">
         <v>43903</v>
       </c>
-      <c r="C78" s="32"/>
-      <c r="D78" s="33"/>
-      <c r="E78" s="33"/>
-      <c r="F78" s="33"/>
-      <c r="G78" s="36"/>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="22" t="s">
+      <c r="C78" s="31"/>
+      <c r="D78" s="32"/>
+      <c r="E78" s="32"/>
+      <c r="F78" s="32"/>
+      <c r="G78" s="31"/>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B79" s="31" t="n">
+      <c r="B79" s="30" t="n">
         <v>43904</v>
       </c>
-      <c r="C79" s="32"/>
-      <c r="D79" s="33"/>
-      <c r="E79" s="33"/>
-      <c r="F79" s="33"/>
-      <c r="G79" s="36"/>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="22" t="s">
+      <c r="C79" s="31"/>
+      <c r="D79" s="32"/>
+      <c r="E79" s="32"/>
+      <c r="F79" s="32"/>
+      <c r="G79" s="31"/>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B80" s="31" t="n">
+      <c r="B80" s="30" t="n">
         <v>43905</v>
       </c>
-      <c r="C80" s="32"/>
-      <c r="D80" s="33"/>
-      <c r="E80" s="33"/>
-      <c r="F80" s="33"/>
-      <c r="G80" s="36"/>
+      <c r="C80" s="31"/>
+      <c r="D80" s="32"/>
+      <c r="E80" s="32"/>
+      <c r="F80" s="32"/>
+      <c r="G80" s="31"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="54"/>
-      <c r="B81" s="31" t="s">
+      <c r="B81" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C81" s="32"/>
-      <c r="D81" s="33" t="n">
+      <c r="C81" s="31"/>
+      <c r="D81" s="32" t="n">
         <f aca="false">SUM(D74:D80)</f>
-        <v>8.5</v>
-      </c>
-      <c r="E81" s="33" t="n">
+        <v>11</v>
+      </c>
+      <c r="E81" s="32" t="n">
         <f aca="false">SUM(E74:E80)</f>
         <v>0</v>
       </c>
-      <c r="F81" s="33" t="n">
+      <c r="F81" s="32" t="n">
         <f aca="false">SUM(F74:F80)</f>
         <v>0</v>
       </c>
-      <c r="G81" s="33" t="n">
+      <c r="G81" s="35" t="n">
         <f aca="false">SUM(D81:F81)</f>
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="54"/>
       <c r="B82" s="55"/>
       <c r="C82" s="56"/>
       <c r="D82" s="57"/>
       <c r="E82" s="57"/>
       <c r="F82" s="58"/>
-      <c r="G82" s="57"/>
-    </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G82" s="59"/>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="54"/>
-      <c r="B83" s="59"/>
-      <c r="C83" s="60"/>
-      <c r="D83" s="61"/>
-      <c r="E83" s="61"/>
-      <c r="F83" s="62"/>
-      <c r="G83" s="61"/>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="60"/>
+      <c r="C83" s="61"/>
+      <c r="D83" s="62"/>
+      <c r="E83" s="62"/>
+      <c r="F83" s="63"/>
+      <c r="G83" s="56"/>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="54"/>
       <c r="B84" s="55"/>
       <c r="C84" s="56"/>
       <c r="D84" s="57"/>
       <c r="E84" s="57"/>
       <c r="F84" s="58"/>
-      <c r="G84" s="57"/>
-    </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G84" s="59"/>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="54"/>
       <c r="B85" s="55"/>
       <c r="C85" s="56"/>
-      <c r="D85" s="63" t="s">
+      <c r="D85" s="64" t="s">
         <v>120</v>
       </c>
-      <c r="E85" s="63" t="s">
+      <c r="E85" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="F85" s="64" t="s">
+      <c r="F85" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="G85" s="65" t="s">
+      <c r="G85" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="H85" s="35" t="s">
+      <c r="H85" s="34" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="54"/>
-      <c r="B86" s="59"/>
-      <c r="C86" s="60" t="s">
+      <c r="B86" s="60"/>
+      <c r="C86" s="61" t="s">
         <v>123</v>
       </c>
-      <c r="D86" s="64" t="n">
+      <c r="D86" s="65" t="n">
         <f aca="false">SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9)</f>
-        <v>81.5</v>
-      </c>
-      <c r="E86" s="64" t="n">
+        <v>84</v>
+      </c>
+      <c r="E86" s="65" t="n">
         <f aca="false">SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9)</f>
         <v>76.5</v>
       </c>
-      <c r="F86" s="64" t="n">
+      <c r="F86" s="65" t="n">
         <f aca="false">SUM(F82,F73,F65,F57,F49,F41,F33,F25,F17,F9)</f>
         <v>2.5</v>
       </c>
       <c r="G86" s="66" t="n">
         <f aca="false">SUM(D86:F86) + 9</f>
-        <v>169.5</v>
+        <v>172</v>
       </c>
       <c r="H86" s="67" t="n">
         <f aca="false">G86/400</f>
-        <v>0.42375</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="55"/>
       <c r="C87" s="56"/>
       <c r="D87" s="57"/>
       <c r="E87" s="57"/>
       <c r="F87" s="58"/>
-      <c r="G87" s="57"/>
-    </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G87" s="59"/>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="55"/>
       <c r="C88" s="68"/>
       <c r="D88" s="57"/>
       <c r="E88" s="57"/>
-      <c r="F88" s="64" t="s">
+      <c r="F88" s="65" t="s">
         <v>124</v>
       </c>
-      <c r="G88" s="65" t="n">
+      <c r="G88" s="61" t="n">
         <f aca="false">G86*50</f>
-        <v>8475</v>
+        <v>8600</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3647,7 +3647,7 @@
       </c>
       <c r="C104" s="9" t="n">
         <f aca="false">G81</f>
-        <v>8.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3716,9 +3716,6 @@
       </c>
       <c r="C115" s="9"/>
     </row>
-    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <conditionalFormatting sqref="B1:B81">
     <cfRule type="timePeriod" priority="2" timePeriod="today" dxfId="0"/>
@@ -3747,7 +3744,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="13" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="12" width="9.14"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Restructuring code to make more OO
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="139">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -382,6 +382,12 @@
   </si>
   <si>
     <t xml:space="preserve">Improving Detection + Meeting Kaushik + Improving Centroid Detection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:30 – 13:30 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improving Centroid Detection</t>
   </si>
   <si>
     <t xml:space="preserve">Design</t>
@@ -1136,7 +1142,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1343,11 +1349,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="77470976"/>
-        <c:axId val="9002944"/>
+        <c:axId val="42298865"/>
+        <c:axId val="99262725"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="77470976"/>
+        <c:axId val="42298865"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1375,14 +1381,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9002944"/>
+        <c:crossAx val="99262725"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="9002944"/>
+        <c:axId val="99262725"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1447,7 +1453,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77470976"/>
+        <c:crossAx val="42298865"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1480,11 +1486,11 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>1792800</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>350640</xdr:rowOff>
+      <xdr:rowOff>351000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>627840</xdr:colOff>
+      <xdr:colOff>627480</xdr:colOff>
       <xdr:row>76</xdr:row>
       <xdr:rowOff>49680</xdr:rowOff>
     </xdr:to>
@@ -1494,8 +1500,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11089800" y="18259200"/>
-        <a:ext cx="5757120" cy="3079800"/>
+        <a:off x="11089800" y="18259560"/>
+        <a:ext cx="5756760" cy="3079440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1902,7 +1908,7 @@
   <dimension ref="A1:U115"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G76" activeCellId="0" sqref="G76"/>
+      <selection pane="topLeft" activeCell="G78" activeCellId="0" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3379,18 +3385,22 @@
         <v>119</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="20" t="s">
         <v>33</v>
       </c>
       <c r="B77" s="30" t="n">
         <v>43902</v>
       </c>
-      <c r="C77" s="31"/>
+      <c r="C77" s="31" t="s">
+        <v>120</v>
+      </c>
       <c r="D77" s="32"/>
       <c r="E77" s="32"/>
       <c r="F77" s="32"/>
-      <c r="G77" s="40"/>
+      <c r="G77" s="33" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="20" t="s">
@@ -3486,7 +3496,7 @@
       <c r="B85" s="55"/>
       <c r="C85" s="56"/>
       <c r="D85" s="64" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E85" s="64" t="s">
         <v>25</v>
@@ -3495,17 +3505,17 @@
         <v>26</v>
       </c>
       <c r="G85" s="61" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H85" s="34" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="54"/>
       <c r="B86" s="60"/>
       <c r="C86" s="61" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D86" s="65" t="n">
         <f aca="false">SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9)</f>
@@ -3542,7 +3552,7 @@
       <c r="D88" s="57"/>
       <c r="E88" s="57"/>
       <c r="F88" s="65" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G88" s="61" t="n">
         <f aca="false">G86*50</f>
@@ -3554,7 +3564,7 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="9" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C94" s="9" t="s">
         <v>6</v>
@@ -3652,67 +3662,67 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C105" s="9"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="9" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C106" s="9"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="9" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C107" s="9"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C108" s="9"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="9" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C109" s="9"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C110" s="9"/>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C111" s="9"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="9" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C112" s="9"/>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="9" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C113" s="9"/>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C114" s="9"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="9" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C115" s="9"/>
     </row>

</xml_diff>

<commit_message>
Created CVModule and restructured top level module
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -384,10 +384,10 @@
     <t xml:space="preserve">Improving Detection + Meeting Kaushik + Improving Centroid Detection</t>
   </si>
   <si>
-    <t xml:space="preserve">11:30 – 13:30 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Improving Centroid Detection</t>
+    <t xml:space="preserve">11:30 – 13:00 18:30 – 20:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improving code structure</t>
   </si>
   <si>
     <t xml:space="preserve">Design</t>
@@ -1068,15 +1068,9 @@
         <name val="Calibri"/>
         <charset val="1"/>
         <family val="2"/>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF006600"/>
+        <color rgb="FF000000"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -1142,7 +1136,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1308,7 +1302,7 @@
                   <c:v>24.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v/>
@@ -1349,11 +1343,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="42298865"/>
-        <c:axId val="99262725"/>
+        <c:axId val="59125970"/>
+        <c:axId val="80954073"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="42298865"/>
+        <c:axId val="59125970"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1381,14 +1375,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99262725"/>
+        <c:crossAx val="80954073"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99262725"/>
+        <c:axId val="80954073"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1453,7 +1447,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42298865"/>
+        <c:crossAx val="59125970"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1908,7 +1902,7 @@
   <dimension ref="A1:U115"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G78" activeCellId="0" sqref="G78"/>
+      <selection pane="topLeft" activeCell="G76" activeCellId="0" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3385,7 +3379,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="20" t="s">
         <v>33</v>
       </c>
@@ -3395,7 +3389,9 @@
       <c r="C77" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="D77" s="32"/>
+      <c r="D77" s="32" t="n">
+        <v>3</v>
+      </c>
       <c r="E77" s="32"/>
       <c r="F77" s="32"/>
       <c r="G77" s="33" t="s">
@@ -3449,7 +3445,7 @@
       <c r="C81" s="31"/>
       <c r="D81" s="32" t="n">
         <f aca="false">SUM(D74:D80)</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E81" s="32" t="n">
         <f aca="false">SUM(E74:E80)</f>
@@ -3461,7 +3457,7 @@
       </c>
       <c r="G81" s="35" t="n">
         <f aca="false">SUM(D81:F81)</f>
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3519,7 +3515,7 @@
       </c>
       <c r="D86" s="65" t="n">
         <f aca="false">SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9)</f>
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E86" s="65" t="n">
         <f aca="false">SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9)</f>
@@ -3531,11 +3527,11 @@
       </c>
       <c r="G86" s="66" t="n">
         <f aca="false">SUM(D86:F86) + 9</f>
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H86" s="67" t="n">
         <f aca="false">G86/400</f>
-        <v>0.43</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3556,7 +3552,7 @@
       </c>
       <c r="G88" s="61" t="n">
         <f aca="false">G86*50</f>
-        <v>8600</v>
+        <v>8750</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3657,7 +3653,7 @@
       </c>
       <c r="C104" s="9" t="n">
         <f aca="false">G81</f>
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Just some time and journal stuff
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="145">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -105,24 +105,45 @@
     <t xml:space="preserve">Report</t>
   </si>
   <si>
+    <t xml:space="preserve">Wk11</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mon</t>
   </si>
   <si>
     <t xml:space="preserve">Lesson 12 - 13</t>
   </si>
   <si>
+    <t xml:space="preserve">17:00 – 18:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset Pi OS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tue</t>
   </si>
   <si>
     <t xml:space="preserve">Lesson 14(0.5) &amp; Pi Setup(1)</t>
   </si>
   <si>
+    <t xml:space="preserve">10:00 – 12:00 18:30 – 20:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuring Pi + Installing OpenCV4.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wed</t>
   </si>
   <si>
     <t xml:space="preserve">OpenCVSetup(3) &amp; Lesson14(0.5)</t>
   </si>
   <si>
+    <t xml:space="preserve">11:30 – 12:00 12:30:14:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Making system run + Speeding up execution on Pi</t>
+  </si>
+  <si>
     <t xml:space="preserve">Thurs</t>
   </si>
   <si>
@@ -153,6 +174,9 @@
     <t xml:space="preserve">Total</t>
   </si>
   <si>
+    <t xml:space="preserve">Wk12</t>
+  </si>
+  <si>
     <t xml:space="preserve">Premade Car Recognition Model + matlab system</t>
   </si>
   <si>
@@ -168,6 +192,9 @@
     <t xml:space="preserve">Wk3</t>
   </si>
   <si>
+    <t xml:space="preserve">Wk13</t>
+  </si>
+  <si>
     <t xml:space="preserve">Raspi Internet + MatLab-&gt;C++ Porting</t>
   </si>
   <si>
@@ -189,9 +216,6 @@
     <t xml:space="preserve">Oreilly Python</t>
   </si>
   <si>
-    <t xml:space="preserve">NB: ATBS = Automate the Boring Stuff</t>
-  </si>
-  <si>
     <t xml:space="preserve">20:00 - 20:30</t>
   </si>
   <si>
@@ -300,9 +324,6 @@
     <t xml:space="preserve">Introduction</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t xml:space="preserve">Read Paper + Background Subtraction</t>
   </si>
   <si>
@@ -390,6 +411,12 @@
     <t xml:space="preserve">Improving code structure</t>
   </si>
   <si>
+    <t xml:space="preserve">11:30 – 13:30 15:30 – 17:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improving centroid detection + Setting up Pi</t>
+  </si>
+  <si>
     <t xml:space="preserve">Design</t>
   </si>
   <si>
@@ -406,15 +433,6 @@
   </si>
   <si>
     <t xml:space="preserve">Week</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wk11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wk12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wk13</t>
   </si>
   <si>
     <t xml:space="preserve">Wk14</t>
@@ -454,7 +472,7 @@
     <numFmt numFmtId="169" formatCode="D/MM/YYYY"/>
     <numFmt numFmtId="170" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -501,6 +519,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FFD9D9D9"/>
@@ -509,38 +534,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF2E75B6"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FFFFFF00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FFF4B183"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -599,7 +593,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -710,19 +704,6 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
         <color rgb="FF808080"/>
       </left>
@@ -772,7 +753,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="67">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -817,6 +798,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -825,202 +810,186 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1029,23 +998,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1062,7 +1031,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
       <font>
         <name val="Calibri"/>
@@ -1070,7 +1039,21 @@
         <family val="2"/>
         <color rgb="FF000000"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF006600"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <colors>
@@ -1114,8 +1097,8 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFF4B183"/>
-      <rgbColor rgb="FF2E75B6"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
@@ -1136,7 +1119,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1302,7 +1285,7 @@
                   <c:v>24.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v/>
@@ -1343,11 +1326,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="59125970"/>
-        <c:axId val="80954073"/>
+        <c:axId val="48574085"/>
+        <c:axId val="81264952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="59125970"/>
+        <c:axId val="48574085"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1375,14 +1358,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80954073"/>
+        <c:crossAx val="81264952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80954073"/>
+        <c:axId val="81264952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1447,7 +1430,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59125970"/>
+        <c:crossAx val="48574085"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1477,16 +1460,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1792800</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>351000</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3204720</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>102600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>627480</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>49680</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>303120</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>25560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1494,8 +1477,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11089800" y="18259560"/>
-        <a:ext cx="5756760" cy="3079440"/>
+        <a:off x="8461800" y="25056720"/>
+        <a:ext cx="5288400" cy="3077640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1515,7 +1498,7 @@
   </sheetPr>
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1901,8 +1884,8 @@
   </sheetPr>
   <dimension ref="A1:U115"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G76" activeCellId="0" sqref="G76"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1914,55 +1897,74 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="9" width="7.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="8" width="45.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="10" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="9" style="10" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="11" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="12" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="11" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="10" width="14.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="10" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="10" width="31.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="15" style="10" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="12" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="13" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="17"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
+      <c r="H1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="21" t="n">
+      <c r="I1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="21"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="23" t="n">
         <v>43836</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="24"/>
       <c r="E2" s="9" t="n">
         <v>1</v>
       </c>
@@ -1970,30 +1972,41 @@
         <v>1</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="17"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="21" t="n">
+      <c r="I2" s="25" t="n">
+        <v>43906</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="21"/>
+    </row>
+    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="23" t="n">
         <v>43837</v>
       </c>
-      <c r="C3" s="22"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="9" t="n">
         <v>1</v>
       </c>
@@ -2001,30 +2014,41 @@
         <v>0.5</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="19"/>
-      <c r="U3" s="17"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="21" t="n">
+        <v>33</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="25" t="n">
+        <v>43907</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="21"/>
+    </row>
+    <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="23" t="n">
         <v>43838</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="9" t="n">
         <v>3</v>
       </c>
@@ -2032,30 +2056,41 @@
         <v>0.5</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="23"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="17"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="21" t="n">
+        <v>37</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="25" t="n">
+        <v>43908</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="21"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="23" t="n">
         <v>43839</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="9" t="n">
         <v>5</v>
       </c>
@@ -2063,112 +2098,132 @@
         <v>0.5</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="17"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="21" t="n">
+        <v>41</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="25" t="n">
+        <v>43909</v>
+      </c>
+      <c r="J5" s="24"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="21"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="23" t="n">
         <v>43840</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="17"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="21" t="n">
+        <v>43</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="25" t="n">
+        <v>43910</v>
+      </c>
+      <c r="J6" s="24"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="21"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="23" t="n">
         <v>43841</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="9" t="n">
         <v>3</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="17"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="21" t="n">
+        <v>45</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="25" t="n">
+        <v>43911</v>
+      </c>
+      <c r="J7" s="24"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="21"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="23" t="n">
         <v>43842</v>
       </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="9" t="n">
         <v>2</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" s="23"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="17"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="25" t="n">
+        <v>43912</v>
+      </c>
+      <c r="J8" s="24"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="26"/>
+      <c r="U8" s="21"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="28" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D9" s="9" t="n">
         <f aca="false">SUM(D3:D8)</f>
@@ -2186,270 +2241,454 @@
         <f aca="false">SUM(D9:F9)</f>
         <v>18.5</v>
       </c>
-      <c r="I9" s="23"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="17"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="30" t="n">
+      <c r="H9" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="8"/>
+      <c r="K9" s="9" t="n">
+        <f aca="false">SUM(K2:K8)</f>
+        <v>5.5</v>
+      </c>
+      <c r="L9" s="9" t="n">
+        <f aca="false">SUM(L2:L8)</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="9" t="n">
+        <f aca="false">SUM(M2:M8)</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="29" t="n">
+        <f aca="false">SUM(K9:M9)</f>
+        <v>5.5</v>
+      </c>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="26"/>
+      <c r="U9" s="21"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="31" t="n">
         <v>43843</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="32" t="n">
+      <c r="C10" s="32"/>
+      <c r="D10" s="33" t="n">
         <v>4</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="23"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="30" t="n">
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="35" t="n">
+        <v>43913</v>
+      </c>
+      <c r="J10" s="32"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="26"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="31" t="n">
         <v>43844</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="32" t="n">
+      <c r="C11" s="32"/>
+      <c r="D11" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="33" t="s">
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="35" t="n">
+        <v>43914</v>
+      </c>
+      <c r="J11" s="32"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="34"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="31" t="n">
+        <v>43845</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="D12" s="33" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="35" t="n">
+        <v>43915</v>
+      </c>
+      <c r="J12" s="32"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="34"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="31" t="n">
+        <v>43846</v>
+      </c>
+      <c r="C13" s="32"/>
+      <c r="D13" s="33" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="35" t="n">
+        <v>43916</v>
+      </c>
+      <c r="J13" s="32"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="34"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="31" t="n">
+        <v>43847</v>
+      </c>
+      <c r="C14" s="32"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="35" t="n">
+        <v>43917</v>
+      </c>
+      <c r="J14" s="32"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="32"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="22" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="30" t="n">
-        <v>43845</v>
-      </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="34"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="30" t="n">
-        <v>43846</v>
-      </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="32" t="n">
-        <v>4</v>
-      </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="33" t="s">
+      <c r="B15" s="31" t="n">
+        <v>43848</v>
+      </c>
+      <c r="C15" s="32"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" s="35" t="n">
+        <v>43918</v>
+      </c>
+      <c r="J15" s="32"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="32"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="22" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="30" t="n">
-        <v>43847</v>
-      </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="31"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="30" t="n">
-        <v>43848</v>
-      </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="31"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="30" t="n">
+      <c r="B16" s="31" t="n">
         <v>43849</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="31"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" s="35" t="n">
+        <v>43919</v>
+      </c>
+      <c r="J16" s="32"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="32"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32" t="n">
+        <v>55</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="32"/>
+      <c r="D17" s="33" t="n">
         <f aca="false">SUM(D10:D16)</f>
         <v>11</v>
       </c>
-      <c r="E17" s="32" t="n">
+      <c r="E17" s="33" t="n">
         <f aca="false">SUM(E10:E16)</f>
         <v>0</v>
       </c>
-      <c r="F17" s="32" t="n">
+      <c r="F17" s="33" t="n">
         <f aca="false">SUM(F10:F16)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="35" t="n">
+      <c r="G17" s="36" t="n">
         <f aca="false">SUM(D17:F17)</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="21" t="n">
+      <c r="H17" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" s="32"/>
+      <c r="K17" s="9" t="n">
+        <f aca="false">SUM(K10:K16)</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="9" t="n">
+        <f aca="false">SUM(L10:L16)</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="9" t="n">
+        <f aca="false">SUM(M10:M16)</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="29" t="n">
+        <f aca="false">SUM(K17:M17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="23" t="n">
         <v>43850</v>
       </c>
-      <c r="C18" s="22"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="9" t="n">
         <v>3</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>48</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="25" t="n">
+        <v>43920</v>
+      </c>
+      <c r="J18" s="24"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="21" t="n">
+      <c r="A19" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="23" t="n">
         <v>43851</v>
       </c>
-      <c r="C19" s="22" t="s">
-        <v>49</v>
+      <c r="C19" s="24" t="s">
+        <v>58</v>
       </c>
       <c r="D19" s="9" t="n">
         <v>3.5</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="37" t="n">
+        <v>59</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="25" t="n">
+        <v>43921</v>
+      </c>
+      <c r="J19" s="24"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="8"/>
+    </row>
+    <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="38" t="n">
         <v>43852</v>
       </c>
-      <c r="C20" s="22" t="s">
-        <v>51</v>
+      <c r="C20" s="24" t="s">
+        <v>60</v>
       </c>
       <c r="D20" s="9" t="n">
         <v>6</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="55.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="21" t="n">
+        <v>61</v>
+      </c>
+      <c r="H20" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="25" t="n">
+        <v>43922</v>
+      </c>
+      <c r="J20" s="24"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="8"/>
+    </row>
+    <row r="21" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="23" t="n">
         <v>43853</v>
       </c>
-      <c r="C21" s="22" t="s">
-        <v>53</v>
+      <c r="C21" s="24" t="s">
+        <v>62</v>
       </c>
       <c r="E21" s="9" t="n">
         <v>5</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H21" s="38" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="21" t="n">
+        <v>63</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" s="25" t="n">
+        <v>43923</v>
+      </c>
+      <c r="J21" s="24"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="8"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="23" t="n">
         <v>43854</v>
       </c>
-      <c r="C22" s="22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="21" t="n">
+      <c r="C22" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="25" t="n">
+        <v>43924</v>
+      </c>
+      <c r="J22" s="24"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="8"/>
+    </row>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="23" t="n">
         <v>43855</v>
       </c>
-      <c r="C23" s="22"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="21" t="n">
+      <c r="C23" s="24"/>
+      <c r="H23" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="I23" s="25" t="n">
+        <v>43925</v>
+      </c>
+      <c r="J23" s="24"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="8"/>
+    </row>
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="23" t="n">
         <v>43856</v>
       </c>
-      <c r="C24" s="22"/>
+      <c r="C24" s="24"/>
+      <c r="H24" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24" s="25" t="n">
+        <v>43926</v>
+      </c>
+      <c r="J24" s="24"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="28" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D25" s="9" t="n">
         <f aca="false">SUM(D18:D24)</f>
@@ -2463,271 +2702,471 @@
         <f aca="false">SUM(D25:F25)</f>
         <v>17.5</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="30" t="n">
+      <c r="H25" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I25" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="J25" s="8"/>
+      <c r="K25" s="9" t="n">
+        <f aca="false">SUM(K18:K24)</f>
+        <v>0</v>
+      </c>
+      <c r="L25" s="9" t="n">
+        <f aca="false">SUM(L18:L24)</f>
+        <v>0</v>
+      </c>
+      <c r="M25" s="9" t="n">
+        <f aca="false">SUM(M18:M24)</f>
+        <v>0</v>
+      </c>
+      <c r="N25" s="29" t="n">
+        <f aca="false">SUM(K25:M25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="31" t="n">
         <v>43857</v>
       </c>
-      <c r="C26" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32" t="n">
+      <c r="C26" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33" t="n">
         <v>1.5</v>
       </c>
-      <c r="F26" s="32"/>
-      <c r="G26" s="33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="30" t="n">
+      <c r="F26" s="33"/>
+      <c r="G26" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="H26" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="35" t="n">
+        <v>43927</v>
+      </c>
+      <c r="J26" s="32"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="34"/>
+    </row>
+    <row r="27" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="31" t="n">
         <v>43858</v>
       </c>
-      <c r="C27" s="31" t="s">
-        <v>59</v>
+      <c r="C27" s="32" t="s">
+        <v>67</v>
       </c>
       <c r="D27" s="39"/>
-      <c r="E27" s="32" t="n">
+      <c r="E27" s="33" t="n">
         <v>4.5</v>
       </c>
-      <c r="F27" s="32"/>
-      <c r="G27" s="33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="30" t="n">
+      <c r="F27" s="33"/>
+      <c r="G27" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="H27" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I27" s="35" t="n">
+        <v>43928</v>
+      </c>
+      <c r="J27" s="32"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="34"/>
+    </row>
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="31" t="n">
         <v>43859</v>
       </c>
-      <c r="C28" s="31"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="33"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="30" t="n">
+      <c r="C28" s="32"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="I28" s="35" t="n">
+        <v>43929</v>
+      </c>
+      <c r="J28" s="32"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="34"/>
+    </row>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="31" t="n">
         <v>43860</v>
       </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
       <c r="G29" s="40"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="30" t="n">
+      <c r="H29" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I29" s="35" t="n">
+        <v>43930</v>
+      </c>
+      <c r="J29" s="32"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="40"/>
+    </row>
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="31" t="n">
         <v>43861</v>
       </c>
-      <c r="C30" s="31"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="31"/>
-    </row>
-    <row r="31" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="30" t="n">
+      <c r="C30" s="32"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I30" s="35" t="n">
+        <v>43931</v>
+      </c>
+      <c r="J30" s="32"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="32"/>
+    </row>
+    <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="31" t="n">
         <v>43862</v>
       </c>
-      <c r="C31" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32" t="n">
+      <c r="C31" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="F31" s="32"/>
-      <c r="G31" s="31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="30" t="n">
+      <c r="F31" s="33"/>
+      <c r="G31" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="H31" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="I31" s="35" t="n">
+        <v>43932</v>
+      </c>
+      <c r="J31" s="32"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="33"/>
+      <c r="N31" s="32"/>
+    </row>
+    <row r="32" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="31" t="n">
         <v>43863</v>
       </c>
-      <c r="C32" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32" t="n">
+      <c r="C32" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="F32" s="32"/>
-      <c r="G32" s="31" t="s">
-        <v>54</v>
-      </c>
+      <c r="F32" s="33"/>
+      <c r="G32" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="H32" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I32" s="35" t="n">
+        <v>43933</v>
+      </c>
+      <c r="J32" s="32"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="32"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="32" t="n">
+        <v>70</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="32"/>
+      <c r="D33" s="33" t="n">
         <f aca="false">SUM(D26:D32)</f>
         <v>0</v>
       </c>
-      <c r="E33" s="32" t="n">
+      <c r="E33" s="33" t="n">
         <f aca="false">SUM(E26:E32)</f>
         <v>12</v>
       </c>
-      <c r="F33" s="32" t="n">
-        <v>0</v>
-      </c>
-      <c r="G33" s="35" t="n">
+      <c r="F33" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="36" t="n">
         <f aca="false">SUM(D33:F33)</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B34" s="21" t="n">
+      <c r="H33" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="I33" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="J33" s="32"/>
+      <c r="K33" s="9" t="n">
+        <f aca="false">SUM(K26:K32)</f>
+        <v>0</v>
+      </c>
+      <c r="L33" s="9" t="n">
+        <f aca="false">SUM(L26:L32)</f>
+        <v>0</v>
+      </c>
+      <c r="M33" s="9" t="n">
+        <f aca="false">SUM(M26:M32)</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="29" t="n">
+        <f aca="false">SUM(K33:M33)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="23" t="n">
         <v>43864</v>
       </c>
-      <c r="C34" s="22" t="s">
-        <v>63</v>
+      <c r="C34" s="24" t="s">
+        <v>71</v>
       </c>
       <c r="E34" s="9" t="n">
         <v>2</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="21" t="n">
+        <v>63</v>
+      </c>
+      <c r="H34" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I34" s="25" t="n">
+        <v>43934</v>
+      </c>
+      <c r="J34" s="24"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="8"/>
+    </row>
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="23" t="n">
         <v>43865</v>
       </c>
-      <c r="C35" s="22" t="s">
-        <v>64</v>
+      <c r="C35" s="24" t="s">
+        <v>72</v>
       </c>
       <c r="E35" s="9" t="n">
         <v>3</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="21" t="n">
+        <v>63</v>
+      </c>
+      <c r="H35" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I35" s="25" t="n">
+        <v>43935</v>
+      </c>
+      <c r="J35" s="24"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="8"/>
+    </row>
+    <row r="36" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="23" t="n">
         <v>43866</v>
       </c>
-      <c r="C36" s="22" t="s">
-        <v>65</v>
+      <c r="C36" s="24" t="s">
+        <v>73</v>
       </c>
       <c r="E36" s="9" t="n">
         <v>6</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="55.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37" s="21" t="n">
+        <v>63</v>
+      </c>
+      <c r="H36" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="I36" s="25" t="n">
+        <v>43936</v>
+      </c>
+      <c r="J36" s="24"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="8"/>
+    </row>
+    <row r="37" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="23" t="n">
         <v>43867</v>
       </c>
-      <c r="C37" s="22" t="s">
-        <v>66</v>
+      <c r="C37" s="24" t="s">
+        <v>74</v>
       </c>
       <c r="E37" s="9" t="n">
         <v>5</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="21" t="n">
+        <v>75</v>
+      </c>
+      <c r="H37" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I37" s="25" t="n">
+        <v>43937</v>
+      </c>
+      <c r="J37" s="24"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="8"/>
+    </row>
+    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="23" t="n">
         <v>43868</v>
       </c>
-      <c r="C38" s="22" t="s">
-        <v>68</v>
+      <c r="C38" s="24" t="s">
+        <v>76</v>
       </c>
       <c r="E38" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="21" t="n">
+        <v>63</v>
+      </c>
+      <c r="H38" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I38" s="25" t="n">
+        <v>43938</v>
+      </c>
+      <c r="J38" s="24"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="8"/>
+    </row>
+    <row r="39" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="23" t="n">
         <v>43869</v>
       </c>
-      <c r="C39" s="22" t="s">
-        <v>69</v>
+      <c r="C39" s="24" t="s">
+        <v>77</v>
       </c>
       <c r="E39" s="9" t="n">
         <v>2</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40" s="21" t="n">
+        <v>63</v>
+      </c>
+      <c r="H39" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="I39" s="25" t="n">
+        <v>43939</v>
+      </c>
+      <c r="J39" s="24"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="8"/>
+    </row>
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="23" t="n">
         <v>43870</v>
       </c>
-      <c r="C40" s="22" t="s">
-        <v>70</v>
+      <c r="C40" s="24" t="s">
+        <v>78</v>
       </c>
       <c r="E40" s="9" t="n">
         <v>3.5</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>54</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="H40" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I40" s="25" t="n">
+        <v>43940</v>
+      </c>
+      <c r="J40" s="24"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="8"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="28" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D41" s="9" t="n">
         <f aca="false">SUM(D34:D40)</f>
@@ -2741,235 +3180,413 @@
         <f aca="false">SUM(D41:F41)</f>
         <v>22.5</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B42" s="30" t="n">
+      <c r="H41" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="I41" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="J41" s="8"/>
+      <c r="K41" s="9" t="n">
+        <f aca="false">SUM(K34:K40)</f>
+        <v>0</v>
+      </c>
+      <c r="L41" s="9" t="n">
+        <f aca="false">SUM(L34:L40)</f>
+        <v>0</v>
+      </c>
+      <c r="M41" s="9" t="n">
+        <f aca="false">SUM(M34:M40)</f>
+        <v>0</v>
+      </c>
+      <c r="N41" s="29" t="n">
+        <f aca="false">SUM(K41:M41)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" s="31" t="n">
         <v>43871</v>
       </c>
-      <c r="C42" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32" t="n">
+      <c r="C42" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="33"/>
+      <c r="E42" s="33" t="n">
         <v>3.5</v>
       </c>
-      <c r="F42" s="32"/>
-      <c r="G42" s="33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" s="30" t="n">
+      <c r="F42" s="33"/>
+      <c r="G42" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="H42" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I42" s="35" t="n">
+        <v>43941</v>
+      </c>
+      <c r="J42" s="32"/>
+      <c r="K42" s="33"/>
+      <c r="L42" s="33"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="34"/>
+    </row>
+    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" s="31" t="n">
         <v>43872</v>
       </c>
-      <c r="C43" s="31"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="33"/>
-    </row>
-    <row r="44" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B44" s="30" t="n">
+      <c r="C43" s="32"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="34"/>
+      <c r="H43" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I43" s="35" t="n">
+        <v>43942</v>
+      </c>
+      <c r="J43" s="32"/>
+      <c r="K43" s="33"/>
+      <c r="L43" s="33"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="34"/>
+    </row>
+    <row r="44" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" s="31" t="n">
         <v>43873</v>
       </c>
-      <c r="C44" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32" t="n">
+      <c r="C44" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="F44" s="32"/>
-      <c r="G44" s="33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B45" s="30" t="n">
+      <c r="F44" s="33"/>
+      <c r="G44" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="H44" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="I44" s="35" t="n">
+        <v>43943</v>
+      </c>
+      <c r="J44" s="32"/>
+      <c r="K44" s="33"/>
+      <c r="L44" s="33"/>
+      <c r="M44" s="33"/>
+      <c r="N44" s="34"/>
+    </row>
+    <row r="45" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" s="31" t="n">
         <v>43874</v>
       </c>
-      <c r="C45" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32" t="n">
+      <c r="C45" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33" t="n">
         <v>4.5</v>
       </c>
-      <c r="F45" s="32"/>
-      <c r="G45" s="33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B46" s="30" t="n">
+      <c r="F45" s="33"/>
+      <c r="G45" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="H45" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I45" s="35" t="n">
+        <v>43944</v>
+      </c>
+      <c r="J45" s="32"/>
+      <c r="K45" s="33"/>
+      <c r="L45" s="33"/>
+      <c r="M45" s="33"/>
+      <c r="N45" s="34"/>
+    </row>
+    <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="31" t="n">
         <v>43875</v>
       </c>
-      <c r="C46" s="31"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="31"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B47" s="30" t="n">
+      <c r="C46" s="32"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I46" s="35" t="n">
+        <v>43945</v>
+      </c>
+      <c r="J46" s="32"/>
+      <c r="K46" s="33"/>
+      <c r="L46" s="33"/>
+      <c r="M46" s="33"/>
+      <c r="N46" s="32"/>
+    </row>
+    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" s="31" t="n">
         <v>43876</v>
       </c>
-      <c r="C47" s="31"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="31"/>
-    </row>
-    <row r="48" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B48" s="30" t="n">
+      <c r="C47" s="32"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="I47" s="35" t="n">
+        <v>43946</v>
+      </c>
+      <c r="J47" s="32"/>
+      <c r="K47" s="33"/>
+      <c r="L47" s="33"/>
+      <c r="M47" s="33"/>
+      <c r="N47" s="32"/>
+    </row>
+    <row r="48" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="31" t="n">
         <v>43877</v>
       </c>
-      <c r="C48" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32" t="n">
+      <c r="C48" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33" t="n">
         <v>2.5</v>
       </c>
-      <c r="F48" s="32"/>
-      <c r="G48" s="31" t="s">
-        <v>54</v>
-      </c>
+      <c r="F48" s="33"/>
+      <c r="G48" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="H48" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I48" s="35" t="n">
+        <v>43947</v>
+      </c>
+      <c r="J48" s="32"/>
+      <c r="K48" s="33"/>
+      <c r="L48" s="33"/>
+      <c r="M48" s="33"/>
+      <c r="N48" s="32"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="B49" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C49" s="31"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32" t="n">
+        <v>84</v>
+      </c>
+      <c r="B49" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" s="32"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="33" t="n">
         <f aca="false">SUM(E42:E48)</f>
         <v>13.5</v>
       </c>
-      <c r="F49" s="32"/>
-      <c r="G49" s="35" t="n">
+      <c r="F49" s="33"/>
+      <c r="G49" s="36" t="n">
         <f aca="false">SUM(D49,E49,F49)</f>
         <v>13.5</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B50" s="21" t="n">
+      <c r="H49" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="I49" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="J49" s="32"/>
+      <c r="K49" s="9" t="n">
+        <f aca="false">SUM(K42:K48)</f>
+        <v>0</v>
+      </c>
+      <c r="L49" s="9" t="n">
+        <f aca="false">SUM(L42:L48)</f>
+        <v>0</v>
+      </c>
+      <c r="M49" s="9" t="n">
+        <f aca="false">SUM(M42:M48)</f>
+        <v>0</v>
+      </c>
+      <c r="N49" s="29" t="n">
+        <f aca="false">SUM(K49:M49)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50" s="23" t="n">
         <v>43878</v>
       </c>
-      <c r="C50" s="22" t="s">
-        <v>77</v>
+      <c r="C50" s="24" t="s">
+        <v>85</v>
       </c>
       <c r="E50" s="9" t="n">
         <v>2</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B51" s="21" t="n">
+        <v>86</v>
+      </c>
+      <c r="H50" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I50" s="25" t="n">
+        <v>43948</v>
+      </c>
+      <c r="J50" s="24"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="8"/>
+    </row>
+    <row r="51" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" s="23" t="n">
         <v>43879</v>
       </c>
-      <c r="C51" s="22" t="s">
-        <v>79</v>
+      <c r="C51" s="24" t="s">
+        <v>87</v>
       </c>
       <c r="E51" s="9" t="n">
         <v>5</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B52" s="21" t="n">
+        <v>88</v>
+      </c>
+      <c r="H51" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I51" s="25" t="n">
+        <v>43949</v>
+      </c>
+      <c r="J51" s="24"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="8"/>
+    </row>
+    <row r="52" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B52" s="23" t="n">
         <v>43880</v>
       </c>
-      <c r="C52" s="22" t="s">
-        <v>81</v>
+      <c r="C52" s="24" t="s">
+        <v>89</v>
       </c>
       <c r="E52" s="9" t="n">
         <v>4.5</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B53" s="21" t="n">
+        <v>90</v>
+      </c>
+      <c r="H52" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="I52" s="25" t="n">
+        <v>43950</v>
+      </c>
+      <c r="J52" s="24"/>
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
+      <c r="M52" s="9"/>
+      <c r="N52" s="8"/>
+    </row>
+    <row r="53" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53" s="23" t="n">
         <v>43881</v>
       </c>
       <c r="C53" s="41" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="E53" s="9" t="n">
         <v>3</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B54" s="21" t="n">
+        <v>92</v>
+      </c>
+      <c r="H53" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I53" s="25" t="n">
+        <v>43951</v>
+      </c>
+      <c r="J53" s="41"/>
+      <c r="K53" s="9"/>
+      <c r="L53" s="9"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="8"/>
+    </row>
+    <row r="54" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" s="23" t="n">
         <v>43882</v>
       </c>
       <c r="C54" s="41" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="E54" s="9" t="n">
         <v>5</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="20" t="s">
-        <v>37</v>
+        <v>94</v>
+      </c>
+      <c r="H54" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I54" s="25" t="n">
+        <v>43952</v>
+      </c>
+      <c r="J54" s="41"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
+      <c r="N54" s="8"/>
+    </row>
+    <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="B55" s="42" t="n">
         <v>43883</v>
       </c>
       <c r="C55" s="43" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D55" s="44" t="n">
         <v>1</v>
@@ -2977,31 +3594,46 @@
       <c r="E55" s="44"/>
       <c r="F55" s="44"/>
       <c r="G55" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="H55" s="46"/>
-      <c r="I55" s="46"/>
-      <c r="J55" s="46"/>
-      <c r="K55" s="46"/>
-      <c r="L55" s="46"/>
-      <c r="M55" s="46"/>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B56" s="21" t="n">
+        <v>96</v>
+      </c>
+      <c r="H55" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="I55" s="25" t="n">
+        <v>43953</v>
+      </c>
+      <c r="J55" s="43"/>
+      <c r="K55" s="44"/>
+      <c r="L55" s="44"/>
+      <c r="M55" s="44"/>
+      <c r="N55" s="45"/>
+    </row>
+    <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56" s="23" t="n">
         <v>43884</v>
       </c>
-      <c r="C56" s="22"/>
-      <c r="N56" s="47"/>
+      <c r="C56" s="24"/>
+      <c r="H56" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I56" s="25" t="n">
+        <v>43954</v>
+      </c>
+      <c r="J56" s="24"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="8"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="28" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D57" s="9" t="n">
         <f aca="false">SUM(D50:D56)</f>
@@ -3015,295 +3647,478 @@
         <f aca="false">SUM(D57:F57)</f>
         <v>20.5</v>
       </c>
-      <c r="N57" s="47"/>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B58" s="30" t="n">
+      <c r="H57" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="I57" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="J57" s="8"/>
+      <c r="K57" s="9" t="n">
+        <f aca="false">SUM(K50:K56)</f>
+        <v>0</v>
+      </c>
+      <c r="L57" s="9" t="n">
+        <f aca="false">SUM(L50:L56)</f>
+        <v>0</v>
+      </c>
+      <c r="M57" s="9" t="n">
+        <f aca="false">SUM(M50:M56)</f>
+        <v>0</v>
+      </c>
+      <c r="N57" s="29" t="n">
+        <f aca="false">SUM(K57:M57)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B58" s="31" t="n">
         <v>43885</v>
       </c>
-      <c r="C58" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="D58" s="32" t="n">
+      <c r="C58" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D58" s="33" t="n">
         <v>1.5</v>
       </c>
-      <c r="E58" s="32"/>
-      <c r="F58" s="32" t="n">
+      <c r="E58" s="33"/>
+      <c r="F58" s="33" t="n">
         <v>1.5</v>
       </c>
-      <c r="G58" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="I58" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="N58" s="47"/>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B59" s="30" t="n">
+      <c r="G58" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="H58" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I58" s="35" t="n">
+        <v>43955</v>
+      </c>
+      <c r="J58" s="32"/>
+      <c r="K58" s="33"/>
+      <c r="L58" s="33"/>
+      <c r="M58" s="33"/>
+      <c r="N58" s="34"/>
+    </row>
+    <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B59" s="31" t="n">
         <v>43886</v>
       </c>
-      <c r="C59" s="31"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="32" t="n">
+      <c r="C59" s="32"/>
+      <c r="D59" s="33"/>
+      <c r="E59" s="33" t="n">
         <v>0.5</v>
       </c>
-      <c r="F59" s="32"/>
-      <c r="G59" s="33"/>
-      <c r="N59" s="47"/>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B60" s="30" t="n">
+      <c r="F59" s="33"/>
+      <c r="G59" s="34"/>
+      <c r="H59" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I59" s="35" t="n">
+        <v>43956</v>
+      </c>
+      <c r="J59" s="32"/>
+      <c r="K59" s="33"/>
+      <c r="L59" s="33"/>
+      <c r="M59" s="33"/>
+      <c r="N59" s="34"/>
+    </row>
+    <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B60" s="31" t="n">
         <v>43887</v>
       </c>
-      <c r="C60" s="31"/>
-      <c r="D60" s="32" t="n">
+      <c r="C60" s="32"/>
+      <c r="D60" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="E60" s="32" t="n">
+      <c r="E60" s="33" t="n">
         <v>0.5</v>
       </c>
-      <c r="F60" s="32"/>
-      <c r="G60" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="N60" s="47"/>
-    </row>
-    <row r="61" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B61" s="30" t="n">
+      <c r="F60" s="33"/>
+      <c r="G60" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="H60" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="I60" s="35" t="n">
+        <v>43957</v>
+      </c>
+      <c r="J60" s="32"/>
+      <c r="K60" s="33"/>
+      <c r="L60" s="33"/>
+      <c r="M60" s="33"/>
+      <c r="N60" s="34"/>
+    </row>
+    <row r="61" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B61" s="31" t="n">
         <v>43888</v>
       </c>
-      <c r="C61" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="D61" s="32" t="n">
+      <c r="C61" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="D61" s="33" t="n">
         <v>3.5</v>
       </c>
-      <c r="E61" s="32" t="n">
+      <c r="E61" s="33" t="n">
         <v>0.5</v>
       </c>
-      <c r="F61" s="32"/>
+      <c r="F61" s="33"/>
       <c r="G61" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="N61" s="47"/>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B62" s="30" t="n">
+        <v>102</v>
+      </c>
+      <c r="H61" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I61" s="35" t="n">
+        <v>43958</v>
+      </c>
+      <c r="J61" s="32"/>
+      <c r="K61" s="33"/>
+      <c r="L61" s="33"/>
+      <c r="M61" s="33"/>
+      <c r="N61" s="40"/>
+    </row>
+    <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B62" s="31" t="n">
         <v>43889</v>
       </c>
-      <c r="C62" s="31"/>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="31"/>
-      <c r="N62" s="47"/>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B63" s="30" t="n">
+      <c r="C62" s="32"/>
+      <c r="D62" s="33"/>
+      <c r="E62" s="33"/>
+      <c r="F62" s="33"/>
+      <c r="G62" s="32"/>
+      <c r="H62" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I62" s="35" t="n">
+        <v>43959</v>
+      </c>
+      <c r="J62" s="32"/>
+      <c r="K62" s="33"/>
+      <c r="L62" s="33"/>
+      <c r="M62" s="33"/>
+      <c r="N62" s="32"/>
+    </row>
+    <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B63" s="31" t="n">
         <v>43890</v>
       </c>
-      <c r="C63" s="31"/>
-      <c r="D63" s="32"/>
-      <c r="E63" s="32"/>
-      <c r="F63" s="32"/>
-      <c r="G63" s="31"/>
-      <c r="N63" s="47"/>
-    </row>
-    <row r="64" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B64" s="30" t="n">
+      <c r="C63" s="32"/>
+      <c r="D63" s="33"/>
+      <c r="E63" s="33"/>
+      <c r="F63" s="33"/>
+      <c r="G63" s="32"/>
+      <c r="H63" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="I63" s="35" t="n">
+        <v>43960</v>
+      </c>
+      <c r="J63" s="32"/>
+      <c r="K63" s="33"/>
+      <c r="L63" s="33"/>
+      <c r="M63" s="33"/>
+      <c r="N63" s="32"/>
+    </row>
+    <row r="64" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B64" s="31" t="n">
         <v>43891</v>
       </c>
-      <c r="C64" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="D64" s="32" t="n">
+      <c r="C64" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D64" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="E64" s="32"/>
-      <c r="F64" s="32"/>
-      <c r="G64" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="N64" s="47"/>
+      <c r="E64" s="33"/>
+      <c r="F64" s="33"/>
+      <c r="G64" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="H64" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I64" s="35" t="n">
+        <v>43961</v>
+      </c>
+      <c r="J64" s="32"/>
+      <c r="K64" s="33"/>
+      <c r="L64" s="33"/>
+      <c r="M64" s="33"/>
+      <c r="N64" s="32"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="B65" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="C65" s="49"/>
-      <c r="D65" s="50" t="n">
+        <v>105</v>
+      </c>
+      <c r="B65" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="C65" s="47"/>
+      <c r="D65" s="48" t="n">
         <f aca="false">SUM(D58:D64)</f>
         <v>9</v>
       </c>
-      <c r="E65" s="50" t="n">
+      <c r="E65" s="48" t="n">
         <f aca="false">SUM(E58:E64)</f>
         <v>1.5</v>
       </c>
-      <c r="F65" s="50" t="n">
+      <c r="F65" s="48" t="n">
         <f aca="false">SUM(F58:F64)</f>
         <v>1.5</v>
       </c>
-      <c r="G65" s="51" t="n">
+      <c r="G65" s="49" t="n">
         <f aca="false">SUM(D65:F65)</f>
         <v>12</v>
       </c>
-      <c r="H65" s="52"/>
-      <c r="I65" s="52"/>
-      <c r="J65" s="52"/>
-      <c r="K65" s="52"/>
-      <c r="L65" s="52"/>
-      <c r="M65" s="52"/>
-    </row>
-    <row r="66" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B66" s="21" t="n">
+      <c r="H65" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="I65" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="J65" s="47"/>
+      <c r="K65" s="9" t="n">
+        <f aca="false">SUM(K58:K64)</f>
+        <v>0</v>
+      </c>
+      <c r="L65" s="9" t="n">
+        <f aca="false">SUM(L58:L64)</f>
+        <v>0</v>
+      </c>
+      <c r="M65" s="9" t="n">
+        <f aca="false">SUM(M58:M64)</f>
+        <v>0</v>
+      </c>
+      <c r="N65" s="29" t="n">
+        <f aca="false">SUM(K65:M65)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B66" s="23" t="n">
         <v>43892</v>
       </c>
-      <c r="C66" s="22" t="s">
-        <v>99</v>
+      <c r="C66" s="24" t="s">
+        <v>106</v>
       </c>
       <c r="D66" s="9" t="n">
         <v>4.5</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B67" s="21" t="n">
+        <v>107</v>
+      </c>
+      <c r="H66" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I66" s="25" t="n">
+        <v>43962</v>
+      </c>
+      <c r="J66" s="24"/>
+      <c r="K66" s="9"/>
+      <c r="L66" s="9"/>
+      <c r="M66" s="9"/>
+      <c r="N66" s="8"/>
+    </row>
+    <row r="67" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B67" s="23" t="n">
         <v>43893</v>
       </c>
-      <c r="C67" s="22" t="s">
-        <v>101</v>
+      <c r="C67" s="24" t="s">
+        <v>108</v>
       </c>
       <c r="D67" s="9" t="n">
         <v>4.5</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B68" s="21" t="n">
+        <v>109</v>
+      </c>
+      <c r="H67" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I67" s="25" t="n">
+        <v>43963</v>
+      </c>
+      <c r="J67" s="24"/>
+      <c r="K67" s="9"/>
+      <c r="L67" s="9"/>
+      <c r="M67" s="9"/>
+      <c r="N67" s="8"/>
+    </row>
+    <row r="68" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B68" s="23" t="n">
         <v>43894</v>
       </c>
-      <c r="C68" s="22" t="s">
-        <v>103</v>
+      <c r="C68" s="24" t="s">
+        <v>110</v>
       </c>
       <c r="D68" s="9" t="n">
         <v>4</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B69" s="21" t="n">
+        <v>111</v>
+      </c>
+      <c r="H68" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="I68" s="25" t="n">
+        <v>43964</v>
+      </c>
+      <c r="J68" s="24"/>
+      <c r="K68" s="9"/>
+      <c r="L68" s="9"/>
+      <c r="M68" s="9"/>
+      <c r="N68" s="8"/>
+    </row>
+    <row r="69" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B69" s="23" t="n">
         <v>43895</v>
       </c>
-      <c r="C69" s="22" t="s">
-        <v>105</v>
+      <c r="C69" s="24" t="s">
+        <v>112</v>
       </c>
       <c r="D69" s="9" t="n">
         <v>5</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B70" s="21" t="n">
+        <v>113</v>
+      </c>
+      <c r="H69" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I69" s="25" t="n">
+        <v>43965</v>
+      </c>
+      <c r="J69" s="24"/>
+      <c r="K69" s="9"/>
+      <c r="L69" s="9"/>
+      <c r="M69" s="9"/>
+      <c r="N69" s="8"/>
+    </row>
+    <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B70" s="23" t="n">
         <v>43896</v>
       </c>
-      <c r="C70" s="22" t="s">
-        <v>107</v>
+      <c r="C70" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="D70" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B71" s="21" t="n">
+        <v>115</v>
+      </c>
+      <c r="H70" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I70" s="25" t="n">
+        <v>43966</v>
+      </c>
+      <c r="J70" s="24"/>
+      <c r="K70" s="9"/>
+      <c r="L70" s="9"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="8"/>
+    </row>
+    <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B71" s="23" t="n">
         <v>43897</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D71" s="9" t="n">
         <v>1.5</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B72" s="21" t="n">
+        <v>117</v>
+      </c>
+      <c r="H71" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="I71" s="25" t="n">
+        <v>43967</v>
+      </c>
+      <c r="J71" s="8"/>
+      <c r="K71" s="9"/>
+      <c r="L71" s="9"/>
+      <c r="M71" s="9"/>
+      <c r="N71" s="8"/>
+    </row>
+    <row r="72" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B72" s="23" t="n">
         <v>43898</v>
       </c>
-      <c r="C72" s="22" t="s">
-        <v>111</v>
+      <c r="C72" s="24" t="s">
+        <v>118</v>
       </c>
       <c r="D72" s="9" t="n">
         <v>4</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>112</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="H72" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I72" s="25" t="n">
+        <v>43968</v>
+      </c>
+      <c r="J72" s="24"/>
+      <c r="K72" s="9"/>
+      <c r="L72" s="9"/>
+      <c r="M72" s="9"/>
+      <c r="N72" s="8"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="28" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D73" s="9" t="n">
         <f aca="false">SUM(D66:D72)</f>
@@ -3321,246 +4136,373 @@
         <f aca="false">SUM(D73:F73)</f>
         <v>24.5</v>
       </c>
-    </row>
-    <row r="74" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B74" s="30" t="n">
+      <c r="H73" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="I73" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="J73" s="8"/>
+      <c r="K73" s="9" t="n">
+        <f aca="false">SUM(K66:K72)</f>
+        <v>0</v>
+      </c>
+      <c r="L73" s="9" t="n">
+        <f aca="false">SUM(L66:L72)</f>
+        <v>0</v>
+      </c>
+      <c r="M73" s="9" t="n">
+        <f aca="false">SUM(M66:M72)</f>
+        <v>0</v>
+      </c>
+      <c r="N73" s="29" t="n">
+        <f aca="false">SUM(K73:M73)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B74" s="31" t="n">
         <v>43899</v>
       </c>
-      <c r="C74" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="D74" s="32" t="n">
+      <c r="C74" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D74" s="33" t="n">
         <v>4</v>
       </c>
-      <c r="E74" s="32"/>
-      <c r="F74" s="32"/>
-      <c r="G74" s="33" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B75" s="53" t="n">
+      <c r="E74" s="33"/>
+      <c r="F74" s="33"/>
+      <c r="G74" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="H74" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I74" s="35" t="n">
+        <v>43969</v>
+      </c>
+      <c r="J74" s="32"/>
+      <c r="K74" s="33"/>
+      <c r="L74" s="33"/>
+      <c r="M74" s="33"/>
+      <c r="N74" s="34"/>
+    </row>
+    <row r="75" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B75" s="51" t="n">
         <v>43900</v>
       </c>
-      <c r="C75" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="D75" s="32" t="n">
+      <c r="C75" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D75" s="33" t="n">
         <v>2.5</v>
       </c>
-      <c r="E75" s="32"/>
-      <c r="F75" s="32"/>
-      <c r="G75" s="33" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B76" s="30" t="n">
+      <c r="E75" s="33"/>
+      <c r="F75" s="33"/>
+      <c r="G75" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="H75" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I75" s="35" t="n">
+        <v>43970</v>
+      </c>
+      <c r="J75" s="32"/>
+      <c r="K75" s="33"/>
+      <c r="L75" s="33"/>
+      <c r="M75" s="33"/>
+      <c r="N75" s="34"/>
+    </row>
+    <row r="76" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B76" s="31" t="n">
         <v>43901</v>
       </c>
-      <c r="C76" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="D76" s="32" t="n">
+      <c r="C76" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="D76" s="33" t="n">
         <v>4.5</v>
       </c>
-      <c r="E76" s="32"/>
-      <c r="F76" s="32"/>
-      <c r="G76" s="33" t="s">
-        <v>119</v>
-      </c>
+      <c r="E76" s="33"/>
+      <c r="F76" s="33"/>
+      <c r="G76" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="H76" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="I76" s="35" t="n">
+        <v>43971</v>
+      </c>
+      <c r="J76" s="32"/>
+      <c r="K76" s="33"/>
+      <c r="L76" s="33"/>
+      <c r="M76" s="33"/>
+      <c r="N76" s="34"/>
     </row>
     <row r="77" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B77" s="30" t="n">
+      <c r="A77" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B77" s="31" t="n">
         <v>43902</v>
       </c>
-      <c r="C77" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="D77" s="32" t="n">
+      <c r="C77" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="D77" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="E77" s="32"/>
-      <c r="F77" s="32"/>
-      <c r="G77" s="33" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B78" s="30" t="n">
+      <c r="E77" s="33"/>
+      <c r="F77" s="33"/>
+      <c r="G77" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="H77" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I77" s="35" t="n">
+        <v>43972</v>
+      </c>
+      <c r="J77" s="32"/>
+      <c r="K77" s="33"/>
+      <c r="L77" s="33"/>
+      <c r="M77" s="33"/>
+      <c r="N77" s="34"/>
+    </row>
+    <row r="78" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B78" s="31" t="n">
         <v>43903</v>
       </c>
-      <c r="C78" s="31"/>
-      <c r="D78" s="32"/>
-      <c r="E78" s="32"/>
-      <c r="F78" s="32"/>
-      <c r="G78" s="31"/>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B79" s="30" t="n">
+      <c r="C78" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="D78" s="33" t="n">
+        <v>4</v>
+      </c>
+      <c r="E78" s="33"/>
+      <c r="F78" s="33"/>
+      <c r="G78" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="H78" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I78" s="35" t="n">
+        <v>43973</v>
+      </c>
+      <c r="J78" s="32"/>
+      <c r="K78" s="33"/>
+      <c r="L78" s="33"/>
+      <c r="M78" s="33"/>
+      <c r="N78" s="32"/>
+    </row>
+    <row r="79" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B79" s="31" t="n">
         <v>43904</v>
       </c>
-      <c r="C79" s="31"/>
-      <c r="D79" s="32"/>
-      <c r="E79" s="32"/>
-      <c r="F79" s="32"/>
-      <c r="G79" s="31"/>
-    </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B80" s="30" t="n">
+      <c r="C79" s="32"/>
+      <c r="D79" s="33"/>
+      <c r="E79" s="33"/>
+      <c r="F79" s="33"/>
+      <c r="G79" s="32"/>
+      <c r="H79" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="I79" s="35" t="n">
+        <v>43974</v>
+      </c>
+      <c r="J79" s="32"/>
+      <c r="K79" s="33"/>
+      <c r="L79" s="33"/>
+      <c r="M79" s="33"/>
+      <c r="N79" s="32"/>
+    </row>
+    <row r="80" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B80" s="31" t="n">
         <v>43905</v>
       </c>
-      <c r="C80" s="31"/>
-      <c r="D80" s="32"/>
-      <c r="E80" s="32"/>
-      <c r="F80" s="32"/>
-      <c r="G80" s="31"/>
+      <c r="C80" s="32"/>
+      <c r="D80" s="33"/>
+      <c r="E80" s="33"/>
+      <c r="F80" s="33"/>
+      <c r="G80" s="32"/>
+      <c r="H80" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I80" s="35" t="n">
+        <v>43975</v>
+      </c>
+      <c r="J80" s="32"/>
+      <c r="K80" s="33"/>
+      <c r="L80" s="33"/>
+      <c r="M80" s="33"/>
+      <c r="N80" s="32"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="54"/>
-      <c r="B81" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C81" s="31"/>
-      <c r="D81" s="32" t="n">
+      <c r="A81" s="52"/>
+      <c r="B81" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C81" s="32"/>
+      <c r="D81" s="33" t="n">
         <f aca="false">SUM(D74:D80)</f>
-        <v>14</v>
-      </c>
-      <c r="E81" s="32" t="n">
+        <v>18</v>
+      </c>
+      <c r="E81" s="33" t="n">
         <f aca="false">SUM(E74:E80)</f>
         <v>0</v>
       </c>
-      <c r="F81" s="32" t="n">
+      <c r="F81" s="33" t="n">
         <f aca="false">SUM(F74:F80)</f>
         <v>0</v>
       </c>
-      <c r="G81" s="35" t="n">
+      <c r="G81" s="36" t="n">
         <f aca="false">SUM(D81:F81)</f>
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="H81" s="52"/>
+      <c r="I81" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="J81" s="32"/>
+      <c r="K81" s="9" t="n">
+        <f aca="false">SUM(K74:K80)</f>
+        <v>0</v>
+      </c>
+      <c r="L81" s="9" t="n">
+        <f aca="false">SUM(L74:L80)</f>
+        <v>0</v>
+      </c>
+      <c r="M81" s="9" t="n">
+        <f aca="false">SUM(M74:M80)</f>
+        <v>0</v>
+      </c>
+      <c r="N81" s="29" t="n">
+        <f aca="false">SUM(K81:M81)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="54"/>
-      <c r="B82" s="55"/>
-      <c r="C82" s="56"/>
-      <c r="D82" s="57"/>
-      <c r="E82" s="57"/>
-      <c r="F82" s="58"/>
-      <c r="G82" s="59"/>
+      <c r="A82" s="52"/>
+      <c r="B82" s="53"/>
+      <c r="C82" s="54"/>
+      <c r="D82" s="55"/>
+      <c r="E82" s="55"/>
+      <c r="F82" s="56"/>
+      <c r="G82" s="57"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="54"/>
-      <c r="B83" s="60"/>
-      <c r="C83" s="61"/>
-      <c r="D83" s="62"/>
-      <c r="E83" s="62"/>
-      <c r="F83" s="63"/>
-      <c r="G83" s="56"/>
+      <c r="A83" s="52"/>
+      <c r="B83" s="30"/>
+      <c r="C83" s="58"/>
+      <c r="D83" s="59"/>
+      <c r="E83" s="59"/>
+      <c r="F83" s="60"/>
+      <c r="G83" s="54"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="54"/>
-      <c r="B84" s="55"/>
-      <c r="C84" s="56"/>
-      <c r="D84" s="57"/>
-      <c r="E84" s="57"/>
-      <c r="F84" s="58"/>
-      <c r="G84" s="59"/>
+      <c r="A84" s="52"/>
+      <c r="B84" s="53"/>
+      <c r="C84" s="54"/>
+      <c r="D84" s="55"/>
+      <c r="E84" s="55"/>
+      <c r="F84" s="56"/>
+      <c r="G84" s="57"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="54"/>
-      <c r="B85" s="55"/>
-      <c r="C85" s="56"/>
-      <c r="D85" s="64" t="s">
-        <v>122</v>
-      </c>
-      <c r="E85" s="64" t="s">
+      <c r="A85" s="52"/>
+      <c r="B85" s="53"/>
+      <c r="C85" s="54"/>
+      <c r="D85" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="E85" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F85" s="65" t="s">
+      <c r="F85" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="G85" s="61" t="s">
-        <v>123</v>
-      </c>
-      <c r="H85" s="34" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="54"/>
-      <c r="B86" s="60"/>
-      <c r="C86" s="61" t="s">
-        <v>125</v>
-      </c>
-      <c r="D86" s="65" t="n">
-        <f aca="false">SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9)</f>
-        <v>87</v>
-      </c>
-      <c r="E86" s="65" t="n">
-        <f aca="false">SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9)</f>
+      <c r="G85" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="H85" s="62" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="52"/>
+      <c r="B86" s="30"/>
+      <c r="C86" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="D86" s="61" t="n">
+        <f aca="false">SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81)</f>
+        <v>96.5</v>
+      </c>
+      <c r="E86" s="61" t="n">
+        <f aca="false">SUM(E81,E73,E65,E57,E49,E41,E33,E25,E17,E9,L9,L17,L25,L33,L41,L49,L57,L65,L73,L81)</f>
         <v>76.5</v>
       </c>
-      <c r="F86" s="65" t="n">
-        <f aca="false">SUM(F82,F73,F65,F57,F49,F41,F33,F25,F17,F9)</f>
+      <c r="F86" s="61" t="n">
+        <f aca="false">SUM(F82,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81)</f>
         <v>2.5</v>
       </c>
-      <c r="G86" s="66" t="n">
+      <c r="G86" s="63" t="n">
         <f aca="false">SUM(D86:F86) + 9</f>
-        <v>175</v>
-      </c>
-      <c r="H86" s="67" t="n">
+        <v>184.5</v>
+      </c>
+      <c r="H86" s="64" t="n">
         <f aca="false">G86/400</f>
-        <v>0.4375</v>
+        <v>0.46125</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="55"/>
-      <c r="C87" s="56"/>
-      <c r="D87" s="57"/>
-      <c r="E87" s="57"/>
-      <c r="F87" s="58"/>
-      <c r="G87" s="59"/>
+      <c r="B87" s="53"/>
+      <c r="C87" s="54"/>
+      <c r="D87" s="55"/>
+      <c r="E87" s="55"/>
+      <c r="F87" s="56"/>
+      <c r="G87" s="57"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="55"/>
-      <c r="C88" s="68"/>
-      <c r="D88" s="57"/>
-      <c r="E88" s="57"/>
-      <c r="F88" s="65" t="s">
-        <v>126</v>
-      </c>
-      <c r="G88" s="61" t="n">
+      <c r="B88" s="53"/>
+      <c r="C88" s="65"/>
+      <c r="D88" s="55"/>
+      <c r="E88" s="55"/>
+      <c r="F88" s="61" t="s">
+        <v>135</v>
+      </c>
+      <c r="G88" s="58" t="n">
         <f aca="false">G86*50</f>
-        <v>8750</v>
+        <v>9225</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="69"/>
+      <c r="B89" s="66"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="9" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="C94" s="9" t="s">
         <v>6</v>
@@ -3577,7 +4519,7 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="9" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C96" s="9" t="n">
         <f aca="false">G17</f>
@@ -3586,7 +4528,7 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="9" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C97" s="9" t="n">
         <f aca="false">G25</f>
@@ -3595,7 +4537,7 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="9" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C98" s="9" t="n">
         <f aca="false">G33</f>
@@ -3604,7 +4546,7 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="9" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C99" s="9" t="n">
         <f aca="false">G41</f>
@@ -3613,7 +4555,7 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="9" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C100" s="9" t="n">
         <f aca="false">G49</f>
@@ -3622,7 +4564,7 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="9" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C101" s="9" t="n">
         <f aca="false">G57</f>
@@ -3631,7 +4573,7 @@
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="9" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C102" s="9" t="n">
         <f aca="false">G65</f>
@@ -3640,7 +4582,7 @@
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="9" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C103" s="9" t="n">
         <f aca="false">G73</f>
@@ -3649,82 +4591,85 @@
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="9" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="C104" s="9" t="n">
         <f aca="false">G81</f>
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="9" t="s">
-        <v>128</v>
+        <v>27</v>
       </c>
       <c r="C105" s="9"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="9" t="s">
-        <v>129</v>
+        <v>50</v>
       </c>
       <c r="C106" s="9"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="9" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
       <c r="C107" s="9"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="9" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C108" s="9"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="9" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C109" s="9"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="9" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C110" s="9"/>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="9" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C111" s="9"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="9" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C112" s="9"/>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="9" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C113" s="9"/>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="9" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C114" s="9"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="9" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C115" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B81">
     <cfRule type="timePeriod" priority="2" timePeriod="today" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I81">
+    <cfRule type="timePeriod" priority="3" timePeriod="today" dxfId="1"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3744,13 +4689,13 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="12" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="13" width="9.14"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Added to small amount of graphics to report
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="156">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -210,6 +210,12 @@
     <t xml:space="preserve">MatLab Tracking Programs</t>
   </si>
   <si>
+    <t xml:space="preserve">12:00 – 13:00 14:00 – 15:30 18:00 – 19:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report Writing + Editing Graphics</t>
+  </si>
+  <si>
     <t xml:space="preserve">N/A</t>
   </si>
   <si>
@@ -454,6 +460,9 @@
   </si>
   <si>
     <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average </t>
   </si>
   <si>
     <t xml:space="preserve">Week</t>
@@ -496,13 +505,12 @@
     <numFmt numFmtId="169" formatCode="D/MM/YYYY"/>
     <numFmt numFmtId="170" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -521,11 +529,87 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -533,21 +617,18 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFD9D9D9"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -555,13 +636,11 @@
       <color rgb="FFD9D9D9"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="13"/>
@@ -579,12 +658,54 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFE7E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF0D0D0D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF8497B0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -606,14 +727,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF0D0D0D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF3B3838"/>
-        <bgColor rgb="FF404040"/>
+        <bgColor rgb="FF333333"/>
       </patternFill>
     </fill>
   </fills>
@@ -623,19 +738,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF595959"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF595959"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF595959"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -650,6 +752,19 @@
       </top>
       <bottom style="thin">
         <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF595959"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF595959"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF595959"/>
       </bottom>
       <diagonal/>
     </border>
@@ -752,7 +867,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -776,17 +891,68 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="68">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -794,276 +960,292 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="11" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="19" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="18" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="18" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="19" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="18" fillId="11" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="18" fillId="11" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="11" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="11" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="18" fillId="12" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="18" fillId="12" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="12" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="12" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="19" fillId="12" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="21" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="10" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="19" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="19" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="19" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
         <name val="Calibri"/>
-        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF000000"/>
       </font>
@@ -1072,7 +1254,6 @@
     <dxf>
       <font>
         <name val="Calibri"/>
-        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF000000"/>
       </font>
@@ -1083,24 +1264,24 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFE7E6E6"/>
-      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -1114,13 +1295,13 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1132,17 +1313,17 @@
       <rgbColor rgb="FF004586"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF0D0D0D"/>
-      <rgbColor rgb="FF404040"/>
+      <rgbColor rgb="FF3B3838"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF3B3838"/>
+      <rgbColor rgb="FF404040"/>
+      <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1349,11 +1530,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="50697372"/>
-        <c:axId val="33367967"/>
+        <c:axId val="22192568"/>
+        <c:axId val="80745241"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50697372"/>
+        <c:axId val="22192568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1381,14 +1562,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33367967"/>
+        <c:crossAx val="80745241"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="33367967"/>
+        <c:axId val="80745241"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1453,7 +1634,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50697372"/>
+        <c:crossAx val="22192568"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1483,16 +1664,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>2440080</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>19800</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>621000</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>93240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>829440</xdr:colOff>
-      <xdr:row>108</xdr:row>
-      <xdr:rowOff>114840</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1364760</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>12240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1500,8 +1681,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7697160" y="20537280"/>
-        <a:ext cx="5287320" cy="3074400"/>
+        <a:off x="11963880" y="19161000"/>
+        <a:ext cx="5287680" cy="3073680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1907,8 +2088,8 @@
   </sheetPr>
   <dimension ref="A1:U115"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A71" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D91" activeCellId="0" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2384,7 +2565,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
         <v>36</v>
       </c>
@@ -2406,11 +2587,17 @@
       <c r="I12" s="36" t="n">
         <v>43915</v>
       </c>
-      <c r="J12" s="33"/>
+      <c r="J12" s="33" t="s">
+        <v>62</v>
+      </c>
       <c r="K12" s="34"/>
       <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="35"/>
+      <c r="M12" s="34" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="N12" s="35" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="23" t="s">
@@ -2426,7 +2613,7 @@
       <c r="E13" s="34"/>
       <c r="F13" s="34"/>
       <c r="G13" s="35" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H13" s="23" t="s">
         <v>40</v>
@@ -2514,7 +2701,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B17" s="32" t="s">
         <v>55</v>
@@ -2537,7 +2724,7 @@
         <v>11</v>
       </c>
       <c r="H17" s="29" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I17" s="36" t="s">
         <v>55</v>
@@ -2553,11 +2740,11 @@
       </c>
       <c r="M17" s="9" t="n">
         <f aca="false">SUM(M10:M16)</f>
-        <v>4</v>
+        <v>6.5</v>
       </c>
       <c r="N17" s="30" t="n">
         <f aca="false">SUM(K17:M17)</f>
-        <v>4</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2572,7 +2759,7 @@
         <v>3</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H18" s="23" t="s">
         <v>28</v>
@@ -2594,13 +2781,13 @@
         <v>43851</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D19" s="9" t="n">
         <v>3.5</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H19" s="23" t="s">
         <v>32</v>
@@ -2622,13 +2809,13 @@
         <v>43852</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D20" s="9" t="n">
         <v>6</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H20" s="38" t="s">
         <v>36</v>
@@ -2650,13 +2837,13 @@
         <v>43853</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E21" s="9" t="n">
         <v>5</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H21" s="23" t="s">
         <v>40</v>
@@ -2678,7 +2865,7 @@
         <v>43854</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H22" s="23" t="s">
         <v>44</v>
@@ -2734,7 +2921,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="29" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>55</v>
@@ -2752,7 +2939,7 @@
         <v>17.5</v>
       </c>
       <c r="H25" s="29" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I25" s="31" t="s">
         <v>55</v>
@@ -2783,7 +2970,7 @@
         <v>43857</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D26" s="34"/>
       <c r="E26" s="34" t="n">
@@ -2791,7 +2978,7 @@
       </c>
       <c r="F26" s="34"/>
       <c r="G26" s="35" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H26" s="23" t="s">
         <v>28</v>
@@ -2813,7 +3000,7 @@
         <v>43858</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D27" s="40"/>
       <c r="E27" s="34" t="n">
@@ -2821,7 +3008,7 @@
       </c>
       <c r="F27" s="34"/>
       <c r="G27" s="35" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H27" s="23" t="s">
         <v>32</v>
@@ -2915,7 +3102,7 @@
         <v>43862</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D31" s="34"/>
       <c r="E31" s="34" t="n">
@@ -2923,7 +3110,7 @@
       </c>
       <c r="F31" s="34"/>
       <c r="G31" s="33" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H31" s="23" t="s">
         <v>48</v>
@@ -2945,7 +3132,7 @@
         <v>43863</v>
       </c>
       <c r="C32" s="33" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D32" s="34"/>
       <c r="E32" s="34" t="n">
@@ -2953,7 +3140,7 @@
       </c>
       <c r="F32" s="34"/>
       <c r="G32" s="33" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H32" s="23" t="s">
         <v>52</v>
@@ -2969,7 +3156,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="29" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B33" s="32" t="s">
         <v>55</v>
@@ -2991,7 +3178,7 @@
         <v>12</v>
       </c>
       <c r="H33" s="29" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I33" s="36" t="s">
         <v>55</v>
@@ -3022,13 +3209,13 @@
         <v>43864</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E34" s="9" t="n">
         <v>2</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H34" s="23" t="s">
         <v>28</v>
@@ -3050,13 +3237,13 @@
         <v>43865</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E35" s="9" t="n">
         <v>3</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H35" s="23" t="s">
         <v>32</v>
@@ -3078,13 +3265,13 @@
         <v>43866</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E36" s="9" t="n">
         <v>6</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H36" s="23" t="s">
         <v>36</v>
@@ -3106,13 +3293,13 @@
         <v>43867</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E37" s="9" t="n">
         <v>5</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H37" s="23" t="s">
         <v>40</v>
@@ -3134,13 +3321,13 @@
         <v>43868</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E38" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H38" s="23" t="s">
         <v>44</v>
@@ -3162,13 +3349,13 @@
         <v>43869</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E39" s="9" t="n">
         <v>2</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H39" s="23" t="s">
         <v>48</v>
@@ -3190,13 +3377,13 @@
         <v>43870</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E40" s="9" t="n">
         <v>3.5</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H40" s="23" t="s">
         <v>52</v>
@@ -3212,7 +3399,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="29" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>55</v>
@@ -3230,7 +3417,7 @@
         <v>22.5</v>
       </c>
       <c r="H41" s="29" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I41" s="31" t="s">
         <v>55</v>
@@ -3261,7 +3448,7 @@
         <v>43871</v>
       </c>
       <c r="C42" s="33" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D42" s="34"/>
       <c r="E42" s="34" t="n">
@@ -3269,7 +3456,7 @@
       </c>
       <c r="F42" s="34"/>
       <c r="G42" s="35" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H42" s="23" t="s">
         <v>28</v>
@@ -3315,7 +3502,7 @@
         <v>43873</v>
       </c>
       <c r="C44" s="33" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D44" s="34"/>
       <c r="E44" s="34" t="n">
@@ -3323,7 +3510,7 @@
       </c>
       <c r="F44" s="34"/>
       <c r="G44" s="35" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H44" s="23" t="s">
         <v>36</v>
@@ -3345,7 +3532,7 @@
         <v>43874</v>
       </c>
       <c r="C45" s="33" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D45" s="34"/>
       <c r="E45" s="34" t="n">
@@ -3353,7 +3540,7 @@
       </c>
       <c r="F45" s="34"/>
       <c r="G45" s="35" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H45" s="23" t="s">
         <v>40</v>
@@ -3423,7 +3610,7 @@
         <v>43877</v>
       </c>
       <c r="C48" s="33" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D48" s="34"/>
       <c r="E48" s="34" t="n">
@@ -3431,7 +3618,7 @@
       </c>
       <c r="F48" s="34"/>
       <c r="G48" s="33" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H48" s="23" t="s">
         <v>52</v>
@@ -3447,7 +3634,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="29" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B49" s="32" t="s">
         <v>55</v>
@@ -3464,7 +3651,7 @@
         <v>13.5</v>
       </c>
       <c r="H49" s="29" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I49" s="36" t="s">
         <v>55</v>
@@ -3495,13 +3682,13 @@
         <v>43878</v>
       </c>
       <c r="C50" s="25" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E50" s="9" t="n">
         <v>2</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H50" s="23" t="s">
         <v>28</v>
@@ -3523,13 +3710,13 @@
         <v>43879</v>
       </c>
       <c r="C51" s="25" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E51" s="9" t="n">
         <v>5</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H51" s="23" t="s">
         <v>32</v>
@@ -3551,13 +3738,13 @@
         <v>43880</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E52" s="9" t="n">
         <v>4.5</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H52" s="23" t="s">
         <v>36</v>
@@ -3579,13 +3766,13 @@
         <v>43881</v>
       </c>
       <c r="C53" s="42" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E53" s="9" t="n">
         <v>3</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H53" s="23" t="s">
         <v>40</v>
@@ -3607,13 +3794,13 @@
         <v>43882</v>
       </c>
       <c r="C54" s="42" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E54" s="9" t="n">
         <v>5</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H54" s="23" t="s">
         <v>44</v>
@@ -3635,7 +3822,7 @@
         <v>43883</v>
       </c>
       <c r="C55" s="44" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D55" s="45" t="n">
         <v>1</v>
@@ -3643,7 +3830,7 @@
       <c r="E55" s="45"/>
       <c r="F55" s="45"/>
       <c r="G55" s="46" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H55" s="23" t="s">
         <v>48</v>
@@ -3679,7 +3866,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="29" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>55</v>
@@ -3697,7 +3884,7 @@
         <v>20.5</v>
       </c>
       <c r="H57" s="29" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I57" s="31" t="s">
         <v>55</v>
@@ -3728,7 +3915,7 @@
         <v>43885</v>
       </c>
       <c r="C58" s="33" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D58" s="34" t="n">
         <v>1.5</v>
@@ -3738,7 +3925,7 @@
         <v>1.5</v>
       </c>
       <c r="G58" s="35" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H58" s="23" t="s">
         <v>28</v>
@@ -3794,7 +3981,7 @@
       </c>
       <c r="F60" s="34"/>
       <c r="G60" s="35" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H60" s="23" t="s">
         <v>36</v>
@@ -3816,7 +4003,7 @@
         <v>43888</v>
       </c>
       <c r="C61" s="33" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D61" s="34" t="n">
         <v>3.5</v>
@@ -3826,7 +4013,7 @@
       </c>
       <c r="F61" s="34"/>
       <c r="G61" s="41" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H61" s="23" t="s">
         <v>40</v>
@@ -3896,7 +4083,7 @@
         <v>43891</v>
       </c>
       <c r="C64" s="33" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D64" s="34" t="n">
         <v>3</v>
@@ -3904,7 +4091,7 @@
       <c r="E64" s="34"/>
       <c r="F64" s="34"/>
       <c r="G64" s="33" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H64" s="23" t="s">
         <v>52</v>
@@ -3920,7 +4107,7 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="29" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B65" s="47" t="s">
         <v>55</v>
@@ -3943,7 +4130,7 @@
         <v>12</v>
       </c>
       <c r="H65" s="29" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I65" s="51" t="s">
         <v>55</v>
@@ -3974,13 +4161,13 @@
         <v>43892</v>
       </c>
       <c r="C66" s="25" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D66" s="9" t="n">
         <v>4.5</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H66" s="23" t="s">
         <v>28</v>
@@ -4002,13 +4189,13 @@
         <v>43893</v>
       </c>
       <c r="C67" s="25" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D67" s="9" t="n">
         <v>4.5</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H67" s="23" t="s">
         <v>32</v>
@@ -4030,13 +4217,13 @@
         <v>43894</v>
       </c>
       <c r="C68" s="25" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D68" s="9" t="n">
         <v>4</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H68" s="23" t="s">
         <v>36</v>
@@ -4058,13 +4245,13 @@
         <v>43895</v>
       </c>
       <c r="C69" s="25" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D69" s="9" t="n">
         <v>5</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H69" s="23" t="s">
         <v>40</v>
@@ -4086,13 +4273,13 @@
         <v>43896</v>
       </c>
       <c r="C70" s="25" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D70" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H70" s="23" t="s">
         <v>44</v>
@@ -4114,13 +4301,13 @@
         <v>43897</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D71" s="9" t="n">
         <v>1.5</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H71" s="23" t="s">
         <v>48</v>
@@ -4142,13 +4329,13 @@
         <v>43898</v>
       </c>
       <c r="C72" s="25" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D72" s="9" t="n">
         <v>4</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H72" s="23" t="s">
         <v>52</v>
@@ -4164,7 +4351,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="29" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>55</v>
@@ -4186,7 +4373,7 @@
         <v>24.5</v>
       </c>
       <c r="H73" s="29" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="I73" s="31" t="s">
         <v>55</v>
@@ -4217,7 +4404,7 @@
         <v>43899</v>
       </c>
       <c r="C74" s="33" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D74" s="34" t="n">
         <v>4</v>
@@ -4225,7 +4412,7 @@
       <c r="E74" s="34"/>
       <c r="F74" s="34"/>
       <c r="G74" s="35" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H74" s="23" t="s">
         <v>28</v>
@@ -4247,7 +4434,7 @@
         <v>43900</v>
       </c>
       <c r="C75" s="33" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D75" s="34" t="n">
         <v>2.5</v>
@@ -4255,7 +4442,7 @@
       <c r="E75" s="34"/>
       <c r="F75" s="34"/>
       <c r="G75" s="35" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H75" s="23" t="s">
         <v>32</v>
@@ -4277,7 +4464,7 @@
         <v>43901</v>
       </c>
       <c r="C76" s="33" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D76" s="34" t="n">
         <v>4.5</v>
@@ -4285,7 +4472,7 @@
       <c r="E76" s="34"/>
       <c r="F76" s="34"/>
       <c r="G76" s="35" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H76" s="23" t="s">
         <v>36</v>
@@ -4307,7 +4494,7 @@
         <v>43902</v>
       </c>
       <c r="C77" s="33" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D77" s="34" t="n">
         <v>3</v>
@@ -4315,7 +4502,7 @@
       <c r="E77" s="34"/>
       <c r="F77" s="34"/>
       <c r="G77" s="35" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H77" s="23" t="s">
         <v>40</v>
@@ -4337,7 +4524,7 @@
         <v>43903</v>
       </c>
       <c r="C78" s="33" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D78" s="34" t="n">
         <v>4</v>
@@ -4345,7 +4532,7 @@
       <c r="E78" s="34"/>
       <c r="F78" s="34"/>
       <c r="G78" s="33" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H78" s="23" t="s">
         <v>44</v>
@@ -4483,7 +4670,7 @@
       <c r="B85" s="54"/>
       <c r="C85" s="55"/>
       <c r="D85" s="11" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E85" s="11" t="s">
         <v>25</v>
@@ -4492,17 +4679,17 @@
         <v>26</v>
       </c>
       <c r="G85" s="59" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H85" s="63" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="53"/>
       <c r="B86" s="31"/>
       <c r="C86" s="59" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D86" s="62" t="n">
         <f aca="false">SUM(D81,D73,D65,D57,D49,D41,D33,D25,D17,D9,K9,K17,K25,K33,K41,K49,K57,K65,K73,K81)</f>
@@ -4514,15 +4701,15 @@
       </c>
       <c r="F86" s="62" t="n">
         <f aca="false">SUM(F81,F73,F65,F57,F49,F41,F33,F25,F17,F9,M9,M17,M25,M33,M41,M49,M57,M65,M73,M81)</f>
-        <v>16</v>
+        <v>18.5</v>
       </c>
       <c r="G86" s="64" t="n">
         <f aca="false">SUM(D86:F86) + 9</f>
-        <v>200</v>
+        <v>202.5</v>
       </c>
       <c r="H86" s="65" t="n">
         <f aca="false">G86/400</f>
-        <v>0.5</v>
+        <v>0.50625</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4539,19 +4726,28 @@
       <c r="D88" s="56"/>
       <c r="E88" s="56"/>
       <c r="F88" s="62" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G88" s="59" t="n">
         <f aca="false">G86*50</f>
-        <v>10000</v>
+        <v>10125</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="67"/>
     </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D90" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E90" s="9" t="e">
+        <f aca="false">dateif("2020-01-01",2020-1-2,"d")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="9" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C94" s="9" t="s">
         <v>6</v>
@@ -4577,7 +4773,7 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C97" s="9" t="n">
         <f aca="false">G25</f>
@@ -4586,7 +4782,7 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C98" s="9" t="n">
         <f aca="false">G33</f>
@@ -4595,7 +4791,7 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C99" s="9" t="n">
         <f aca="false">G41</f>
@@ -4604,7 +4800,7 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C100" s="9" t="n">
         <f aca="false">G49</f>
@@ -4613,7 +4809,7 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C101" s="9" t="n">
         <f aca="false">G57</f>
@@ -4622,7 +4818,7 @@
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="9" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C102" s="9" t="n">
         <f aca="false">G65</f>
@@ -4631,7 +4827,7 @@
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="9" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C103" s="9" t="n">
         <f aca="false">G73</f>
@@ -4640,7 +4836,7 @@
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="9" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C104" s="9" t="n">
         <f aca="false">G81</f>
@@ -4664,55 +4860,55 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C107" s="9"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="9" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C108" s="9"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="9" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C109" s="9"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="9" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C110" s="9"/>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="9" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C111" s="9"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="9" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C112" s="9"/>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="9" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C113" s="9"/>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="9" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C114" s="9"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C115" s="9"/>
     </row>

</xml_diff>